<commit_message>
Buildings fleshed out, camera script started
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C562DA-FEDF-4C44-B459-43C5319D571B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF2002C-D089-47C5-80E1-81C063043F27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,26 @@
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
     <sheet name="Buildings" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="66">
   <si>
     <t>Tier</t>
   </si>
@@ -118,10 +127,112 @@
     <t>Watchtower</t>
   </si>
   <si>
-    <t>Lab</t>
-  </si>
-  <si>
     <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Buildable?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Garden</t>
+  </si>
+  <si>
+    <t>Orchard</t>
+  </si>
+  <si>
+    <t>Ranch</t>
+  </si>
+  <si>
+    <t>Hydroponics Tower</t>
+  </si>
+  <si>
+    <t>Raw Production</t>
+  </si>
+  <si>
+    <t>Production With Tier Bonus</t>
+  </si>
+  <si>
+    <t>Numeric Modifier</t>
+  </si>
+  <si>
+    <t>Cottage</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>Condomium</t>
+  </si>
+  <si>
+    <t>Villa</t>
+  </si>
+  <si>
+    <t>Foundry</t>
+  </si>
+  <si>
+    <t>Forge</t>
+  </si>
+  <si>
+    <t>Factory</t>
+  </si>
+  <si>
+    <t>Mill</t>
+  </si>
+  <si>
+    <t>Dormitory</t>
+  </si>
+  <si>
+    <t>Garrison</t>
+  </si>
+  <si>
+    <t>Quarters</t>
+  </si>
+  <si>
+    <t>Headquarters</t>
+  </si>
+  <si>
+    <t>Auto Laser Tower</t>
+  </si>
+  <si>
+    <t>Auto Missile Complex</t>
+  </si>
+  <si>
+    <t>Laser Tower</t>
+  </si>
+  <si>
+    <t>Missile Complex</t>
+  </si>
+  <si>
+    <t>Research College</t>
+  </si>
+  <si>
+    <t>Research Lab</t>
+  </si>
+  <si>
+    <t>Research Institute</t>
+  </si>
+  <si>
+    <t>MultiBrain Complex</t>
+  </si>
+  <si>
+    <t>Quantum Brain</t>
+  </si>
+  <si>
+    <t>Stockpile</t>
+  </si>
+  <si>
+    <t>Depot</t>
+  </si>
+  <si>
+    <t>Distribution Center</t>
+  </si>
+  <si>
+    <t>Storehouse</t>
   </si>
 </sst>
 </file>
@@ -187,11 +298,16 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -475,19 +591,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,8 +614,11 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -508,8 +628,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -519,8 +642,11 @@
       <c r="C3" s="3">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -530,8 +656,11 @@
       <c r="C4" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -541,8 +670,11 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -551,6 +683,9 @@
       </c>
       <c r="C6" s="3">
         <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -561,26 +696,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EF5834-8EEB-44D9-8EA7-D238A22091DC}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -591,25 +729,34 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -617,57 +764,198 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2">
+        <f t="array" ref="E2">SUM(F2:J2)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f t="array" ref="L2">PRODUCT(K2,Tiers!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <f t="array" ref="E3">SUM(F3:J3)</f>
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <f t="array" ref="L3">PRODUCT(K3,Tiers!D3)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <f t="array" ref="E4">SUM(F4:J4)</f>
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f>PRODUCT(K4,Tiers!D4)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <f>SUM(F5:J5)</f>
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f>PRODUCT(K5,Tiers!D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f>PRODUCT(K6,Tiers!D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -677,55 +965,196 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <f>SUM(F7:J7)</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f>PRODUCT(K7,Tiers!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <f>SUM(F8:J8)</f>
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <f>PRODUCT(K8,Tiers!D3)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <f>SUM(F9:J9)</f>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f>PRODUCT(K9,Tiers!D4)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <f>SUM(F10:J10)</f>
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <f>PRODUCT(K10,Tiers!D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <f>PRODUCT(K11,Tiers!D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -735,55 +1164,196 @@
       <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <f>SUM(F12:J12)</f>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f>PRODUCT(K12,Tiers!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <f>SUM(F13:J13)</f>
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <f>PRODUCT(K13,Tiers!D3)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <f>SUM(F14:J14)</f>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <f>PRODUCT(K14,Tiers!D4)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <f>SUM(F15:J15)</f>
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <f>PRODUCT(K15,Tiers!D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f>PRODUCT(K16,Tiers!D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -793,55 +1363,196 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <f>SUM(F17:J17)</f>
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f>PRODUCT(K17,Tiers!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18">
+        <f>SUM(F18:J18)</f>
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <f>PRODUCT(K18,Tiers!D3)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <f>SUM(F19:J19)</f>
+        <v>13</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <f>PRODUCT(K19,Tiers!D4)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <f>SUM(F20:J20)</f>
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <f>PRODUCT(K20,Tiers!D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <f>PRODUCT(K21,Tiers!D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -851,55 +1562,192 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <f>SUM(F22:J22)</f>
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23">
+        <f>SUM(F23:J23)</f>
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <f>SUM(F24:J24)</f>
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <f>SUM(F25:J25)</f>
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <f>SUM(F26:J26)</f>
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -907,57 +1755,198 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27">
+        <f>SUM(F27:J27)</f>
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f>PRODUCT(K27,Tiers!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28">
+        <f>SUM(F28:J28)</f>
+        <v>9</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <f>PRODUCT(K28,Tiers!D3)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29">
+        <f>SUM(F29:J29)</f>
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <f>PRODUCT(K29,Tiers!D4)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30">
+        <f>SUM(F30:J30)</f>
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <f>PRODUCT(K30,Tiers!D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <f>PRODUCT(K31,Tiers!D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -965,57 +1954,198 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32">
+        <f>SUM(F32:J32)</f>
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <f>PRODUCT(K32,Tiers!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <f>SUM(F33:J33)</f>
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <f>PRODUCT(K33,Tiers!D3)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34">
+        <f>SUM(F34:J34)</f>
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>3</v>
+      </c>
+      <c r="L34">
+        <f>PRODUCT(K34,Tiers!D4)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35">
+        <f t="array" ref="E35">SUM(F35:J35)</f>
+        <v>11</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <f>PRODUCT(K35,Tiers!D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>23</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36">
+        <v>5</v>
+      </c>
+      <c r="L36">
+        <f>PRODUCT(K36,Tiers!D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -1026,26 +2156,38 @@
         <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" s="6" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2 E3:E5 E7:E10 E12:E15 E17:E20 E27:E30 E32:E35" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finally fixed the camera, started combat units UI and design work
I am an idiot
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CA9ACB-2721-4AAB-8703-F2DC3A1F78AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B031AA-ABAC-4CC2-8D90-1CFC3AB882CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,7 +346,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -385,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -779,10 +780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EF5834-8EEB-44D9-8EA7-D238A22091DC}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,16 +793,17 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -817,29 +819,30 @@
       <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="22"/>
+    </row>
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -853,17 +856,18 @@
         <v>32</v>
       </c>
       <c r="E2" s="7">
-        <f>L2/L2</f>
+        <f>G2/G2</f>
         <v>1</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6">
-        <v>0</v>
+        <f>PRODUCT(F2,Tiers!D2) + F2</f>
+        <v>1</v>
       </c>
       <c r="H2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="6">
         <v>0</v>
@@ -872,14 +876,13 @@
         <v>0</v>
       </c>
       <c r="K2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="6">
-        <f>PRODUCT(K2,Tiers!D2) + K2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -893,33 +896,33 @@
         <v>32</v>
       </c>
       <c r="E3" s="7">
-        <f>L3/L2</f>
+        <f>G3/G2</f>
         <v>1.25</v>
       </c>
       <c r="F3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <f>PRODUCT(F3,Tiers!D3) + F3</f>
+        <v>1.25</v>
       </c>
       <c r="H3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="6">
-        <f>PRODUCT(K3,Tiers!D3) + K3</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -933,33 +936,33 @@
         <v>32</v>
       </c>
       <c r="E4" s="7">
-        <f>L4/L2</f>
+        <f>G4/G2</f>
         <v>3</v>
       </c>
       <c r="F4" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <f>PRODUCT(F4,Tiers!D4) + F4</f>
+        <v>3</v>
       </c>
       <c r="H4" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L4" s="6">
-        <f>PRODUCT(K4,Tiers!D4) + K4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -973,33 +976,33 @@
         <v>32</v>
       </c>
       <c r="E5" s="7">
-        <f>L5/L2</f>
+        <f>G5/G2</f>
         <v>6</v>
       </c>
       <c r="F5" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <f>PRODUCT(F5,Tiers!D5) + F5</f>
+        <v>6</v>
       </c>
       <c r="H5" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L5" s="6">
-        <f>PRODUCT(K5,Tiers!D5) + K5</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1013,14 +1016,15 @@
         <v>31</v>
       </c>
       <c r="E6" s="7">
-        <f>L6/L2</f>
+        <f>G6/G2</f>
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>24</v>
+      <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <f>PRODUCT(F6,Tiers!D6) + F6</f>
+        <v>15</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>24</v>
@@ -1031,15 +1035,14 @@
       <c r="J6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="6">
-        <v>5</v>
-      </c>
-      <c r="L6" s="6">
-        <f>PRODUCT(K6,Tiers!D6) + K6</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1053,33 +1056,33 @@
         <v>32</v>
       </c>
       <c r="E7" s="9">
-        <f>L7/L7</f>
+        <f>G7/G7</f>
         <v>1</v>
       </c>
       <c r="F7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="8">
+        <f>PRODUCT(F7,Tiers!D2) + F7</f>
         <v>1</v>
       </c>
       <c r="H7" s="8">
         <v>0</v>
       </c>
       <c r="I7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="8">
         <v>0</v>
       </c>
       <c r="K7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="8">
-        <f>PRODUCT(K7,Tiers!D2) + K7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
@@ -1093,33 +1096,33 @@
         <v>32</v>
       </c>
       <c r="E8" s="9">
-        <f>L8/L7</f>
+        <f>G8/G7</f>
         <v>1.25</v>
       </c>
       <c r="F8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="8">
-        <v>2</v>
+        <f>PRODUCT(F8,Tiers!D3) + F8</f>
+        <v>1.25</v>
       </c>
       <c r="H8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="8">
         <v>1</v>
       </c>
       <c r="L8" s="8">
-        <f>PRODUCT(K8,Tiers!D3) + K8</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1133,33 +1136,33 @@
         <v>32</v>
       </c>
       <c r="E9" s="9">
-        <f>L9/L7</f>
+        <f>G9/G7</f>
         <v>3</v>
       </c>
       <c r="F9" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="8">
+        <f>PRODUCT(F9,Tiers!D4) + F9</f>
         <v>3</v>
       </c>
       <c r="H9" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="8">
         <v>2</v>
       </c>
       <c r="L9" s="8">
-        <f>PRODUCT(K9,Tiers!D4) + K9</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -1173,33 +1176,33 @@
         <v>32</v>
       </c>
       <c r="E10" s="9">
-        <f>L10/L7</f>
+        <f>G10/G7</f>
         <v>6</v>
       </c>
       <c r="F10" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" s="8">
-        <v>4</v>
+        <f>PRODUCT(F10,Tiers!D5) + F10</f>
+        <v>6</v>
       </c>
       <c r="H10" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I10" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J10" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="8">
         <v>3</v>
       </c>
       <c r="L10" s="8">
-        <f>PRODUCT(K10,Tiers!D5) + K10</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -1213,14 +1216,15 @@
         <v>31</v>
       </c>
       <c r="E11" s="9">
-        <f>L11/L7</f>
+        <f>G11/G7</f>
         <v>15</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>24</v>
+      <c r="F11" s="8">
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
+        <f>PRODUCT(F11,Tiers!D6)+F11</f>
+        <v>15</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>24</v>
@@ -1231,15 +1235,14 @@
       <c r="J11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="8">
-        <v>5</v>
-      </c>
-      <c r="L11" s="8">
-        <f>PRODUCT(K11,Tiers!D6)+K11</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -1253,17 +1256,18 @@
         <v>32</v>
       </c>
       <c r="E12" s="11">
-        <f>L12/L12</f>
+        <f>G12/G12</f>
         <v>1</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="10">
-        <v>0</v>
+        <f>PRODUCT(F12,Tiers!D2)+F12</f>
+        <v>1</v>
       </c>
       <c r="H12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="10">
         <v>0</v>
@@ -1272,14 +1276,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="10">
-        <f>PRODUCT(K12,Tiers!D2)+K12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -1293,33 +1296,33 @@
         <v>32</v>
       </c>
       <c r="E13" s="11">
-        <f>L13/L12</f>
+        <f>G13/G12</f>
         <v>1.25</v>
       </c>
       <c r="F13" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="10">
-        <v>0</v>
+        <f>PRODUCT(F13,Tiers!D3)+F13</f>
+        <v>1.25</v>
       </c>
       <c r="H13" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="10">
         <v>0</v>
       </c>
       <c r="J13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="10">
-        <f>PRODUCT(K13,Tiers!D3)+K13</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
@@ -1333,33 +1336,33 @@
         <v>32</v>
       </c>
       <c r="E14" s="11">
-        <f>L14/L12</f>
+        <f>G14/G12</f>
         <v>3</v>
       </c>
       <c r="F14" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" s="10">
-        <v>0</v>
+        <f>PRODUCT(F14,Tiers!D4)+F14</f>
+        <v>3</v>
       </c>
       <c r="H14" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" s="10">
         <v>0</v>
       </c>
       <c r="J14" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L14" s="10">
-        <f>PRODUCT(K14,Tiers!D4)+K14</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>17</v>
       </c>
@@ -1373,33 +1376,33 @@
         <v>32</v>
       </c>
       <c r="E15" s="11">
-        <f>L15/L12</f>
+        <f>G15/G12</f>
         <v>6</v>
       </c>
       <c r="F15" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="10">
-        <v>0</v>
+        <f>PRODUCT(F15,Tiers!D5)+F15</f>
+        <v>6</v>
       </c>
       <c r="H15" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="10">
         <v>0</v>
       </c>
       <c r="J15" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K15" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L15" s="10">
-        <f>PRODUCT(K15,Tiers!D5)+K15</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -1413,14 +1416,15 @@
         <v>31</v>
       </c>
       <c r="E16" s="11">
-        <f>L16/L12</f>
+        <f>G16/G12</f>
         <v>15</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>24</v>
+      <c r="F16" s="10">
+        <v>5</v>
+      </c>
+      <c r="G16" s="10">
+        <f>PRODUCT(F16,Tiers!D6)+F16</f>
+        <v>15</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>24</v>
@@ -1431,12 +1435,11 @@
       <c r="J16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="10">
-        <v>5</v>
-      </c>
-      <c r="L16" s="10">
-        <f>PRODUCT(K16,Tiers!D6)+K16</f>
-        <v>15</v>
+      <c r="K16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1453,30 +1456,30 @@
         <v>32</v>
       </c>
       <c r="E17" s="13">
-        <f>L17/L17</f>
+        <f>G17/G17</f>
         <v>1</v>
       </c>
       <c r="F17" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="12">
+        <f>PRODUCT(F17,Tiers!D2)+F17</f>
         <v>1</v>
       </c>
       <c r="H17" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="12">
         <v>1</v>
       </c>
       <c r="J17" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="12">
         <v>1</v>
       </c>
       <c r="L17" s="12">
-        <f>PRODUCT(K17,Tiers!D2)+K17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1493,30 +1496,30 @@
         <v>32</v>
       </c>
       <c r="E18" s="13">
-        <f>L18/L17</f>
+        <f>G18/G17</f>
         <v>1.25</v>
       </c>
       <c r="F18" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18" s="12">
-        <v>2</v>
+        <f>PRODUCT(F18,Tiers!D3)+F18</f>
+        <v>1.25</v>
       </c>
       <c r="H18" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="12">
         <v>2</v>
       </c>
       <c r="J18" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="12">
-        <f>PRODUCT(K18,Tiers!D3)+K18</f>
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1533,30 +1536,30 @@
         <v>32</v>
       </c>
       <c r="E19" s="13">
-        <f>L19/L17</f>
+        <f>G19/G17</f>
         <v>3</v>
       </c>
       <c r="F19" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G19" s="12">
+        <f>PRODUCT(F19,Tiers!D4)+F19</f>
         <v>3</v>
       </c>
       <c r="H19" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I19" s="12">
         <v>3</v>
       </c>
       <c r="J19" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K19" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" s="12">
-        <f>PRODUCT(K19,Tiers!D4)+K19</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1573,30 +1576,30 @@
         <v>32</v>
       </c>
       <c r="E20" s="13">
-        <f>L20/L17</f>
+        <f>G20/G17</f>
         <v>6</v>
       </c>
       <c r="F20" s="12">
+        <v>3</v>
+      </c>
+      <c r="G20" s="12">
+        <f>PRODUCT(F20,Tiers!D5)+F20</f>
+        <v>6</v>
+      </c>
+      <c r="H20" s="12">
         <v>5</v>
       </c>
-      <c r="G20" s="12">
-        <v>4</v>
-      </c>
-      <c r="H20" s="12">
-        <v>4</v>
-      </c>
       <c r="I20" s="12">
         <v>4</v>
       </c>
       <c r="J20" s="12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K20" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L20" s="12">
-        <f>PRODUCT(K20,Tiers!D5)+K20</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1613,14 +1616,15 @@
         <v>31</v>
       </c>
       <c r="E21" s="13">
-        <f>L21/L17</f>
+        <f>G21/G17</f>
         <v>15</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>24</v>
+      <c r="F21" s="12">
+        <v>5</v>
+      </c>
+      <c r="G21" s="12">
+        <f>PRODUCT(F21,Tiers!D6)+F21</f>
+        <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>24</v>
@@ -1631,12 +1635,11 @@
       <c r="J21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K21" s="12">
-        <v>5</v>
-      </c>
-      <c r="L21" s="12">
-        <f>PRODUCT(K21,Tiers!D6)+K21</f>
-        <v>15</v>
+      <c r="K21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1655,26 +1658,26 @@
       <c r="E22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="20">
-        <v>1</v>
-      </c>
-      <c r="G22" s="20">
-        <v>0</v>
+      <c r="F22" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="H22" s="20">
         <v>1</v>
       </c>
       <c r="I22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="20">
         <v>1</v>
       </c>
-      <c r="K22" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="21" t="s">
-        <v>24</v>
+      <c r="K22" s="20">
+        <v>1</v>
+      </c>
+      <c r="L22" s="20">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1693,26 +1696,26 @@
       <c r="E23" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="20">
-        <v>2</v>
-      </c>
-      <c r="G23" s="20">
-        <v>0</v>
+      <c r="F23" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="H23" s="20">
         <v>2</v>
       </c>
       <c r="I23" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23" s="20">
         <v>2</v>
       </c>
-      <c r="K23" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="21" t="s">
-        <v>24</v>
+      <c r="K23" s="20">
+        <v>2</v>
+      </c>
+      <c r="L23" s="20">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1731,26 +1734,26 @@
       <c r="E24" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="20">
-        <v>3</v>
-      </c>
-      <c r="G24" s="20">
-        <v>0</v>
+      <c r="F24" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="H24" s="20">
         <v>3</v>
       </c>
       <c r="I24" s="20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J24" s="20">
         <v>3</v>
       </c>
-      <c r="K24" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>24</v>
+      <c r="K24" s="20">
+        <v>3</v>
+      </c>
+      <c r="L24" s="20">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1769,26 +1772,26 @@
       <c r="E25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="20">
-        <v>0</v>
-      </c>
-      <c r="G25" s="20">
-        <v>0</v>
+      <c r="F25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="H25" s="20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I25" s="20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J25" s="20">
         <v>4</v>
       </c>
-      <c r="K25" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="21" t="s">
-        <v>24</v>
+      <c r="K25" s="20">
+        <v>4</v>
+      </c>
+      <c r="L25" s="20">
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1807,26 +1810,26 @@
       <c r="E26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="20">
-        <v>0</v>
-      </c>
-      <c r="G26" s="20">
-        <v>0</v>
+      <c r="F26" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="H26" s="20">
+        <v>0</v>
+      </c>
+      <c r="I26" s="20">
+        <v>0</v>
+      </c>
+      <c r="J26" s="20">
         <v>6</v>
       </c>
-      <c r="I26" s="20">
+      <c r="K26" s="20">
         <v>6</v>
       </c>
-      <c r="J26" s="20">
-        <v>4</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>24</v>
+      <c r="L26" s="20">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1843,30 +1846,30 @@
         <v>32</v>
       </c>
       <c r="E27" s="15">
-        <f>L27/L27</f>
+        <f>G27/G27</f>
         <v>1</v>
       </c>
       <c r="F27" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="14">
-        <v>0</v>
+        <f>PRODUCT(F27,Tiers!D2)+F27</f>
+        <v>1</v>
       </c>
       <c r="H27" s="14">
         <v>2</v>
       </c>
       <c r="I27" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L27" s="14">
-        <f>PRODUCT(K27,Tiers!D2)+K27</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1883,30 +1886,30 @@
         <v>32</v>
       </c>
       <c r="E28" s="15">
-        <f>L28/L27</f>
+        <f>G28/G27</f>
         <v>1.25</v>
       </c>
       <c r="F28" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28" s="14">
-        <v>0</v>
+        <f>PRODUCT(F28,Tiers!D3)+F28</f>
+        <v>1.25</v>
       </c>
       <c r="H28" s="14">
         <v>3</v>
       </c>
       <c r="I28" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J28" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K28" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L28" s="14">
-        <f>PRODUCT(K28,Tiers!D3)+K28</f>
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1923,30 +1926,30 @@
         <v>32</v>
       </c>
       <c r="E29" s="15">
-        <f>L29/L27</f>
+        <f>G29/G27</f>
         <v>3</v>
       </c>
       <c r="F29" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G29" s="14">
-        <v>0</v>
+        <f>PRODUCT(F29,Tiers!D4)+F29</f>
+        <v>3</v>
       </c>
       <c r="H29" s="14">
         <v>4</v>
       </c>
       <c r="I29" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J29" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K29" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L29" s="14">
-        <f>PRODUCT(K29,Tiers!D4)+K29</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1963,30 +1966,30 @@
         <v>32</v>
       </c>
       <c r="E30" s="15">
-        <f>L30/L27</f>
+        <f>G30/G27</f>
         <v>6</v>
       </c>
       <c r="F30" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G30" s="14">
-        <v>0</v>
+        <f>PRODUCT(F30,Tiers!D5)+F30</f>
+        <v>6</v>
       </c>
       <c r="H30" s="14">
         <v>5</v>
       </c>
       <c r="I30" s="14">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
         <v>5</v>
       </c>
-      <c r="J30" s="14">
-        <v>0</v>
-      </c>
       <c r="K30" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L30" s="14">
-        <f>PRODUCT(K30,Tiers!D5)+K30</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2003,14 +2006,15 @@
         <v>31</v>
       </c>
       <c r="E31" s="15">
-        <f>L31/L27</f>
+        <f>G31/G27</f>
         <v>15</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>24</v>
+      <c r="F31" s="14">
+        <v>5</v>
+      </c>
+      <c r="G31" s="14">
+        <f>PRODUCT(F31,Tiers!D6)+F31</f>
+        <v>15</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>24</v>
@@ -2021,12 +2025,11 @@
       <c r="J31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K31" s="14">
-        <v>5</v>
-      </c>
-      <c r="L31" s="14">
-        <f>PRODUCT(K31,Tiers!D6)+K31</f>
-        <v>15</v>
+      <c r="K31" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2043,20 +2046,21 @@
         <v>32</v>
       </c>
       <c r="E32" s="17">
-        <f>L32/L32</f>
+        <f>G32/G32</f>
         <v>1</v>
       </c>
       <c r="F32" s="16">
         <v>1</v>
       </c>
       <c r="G32" s="16">
-        <v>0</v>
+        <f>PRODUCT(F32,Tiers!D2)+F32</f>
+        <v>1</v>
       </c>
       <c r="H32" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" s="16">
         <v>0</v>
@@ -2065,8 +2069,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="16">
-        <f>PRODUCT(K32,Tiers!D2)+K32</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2083,30 +2086,30 @@
         <v>32</v>
       </c>
       <c r="E33" s="17">
-        <f>L33/L32</f>
+        <f>G33/G32</f>
         <v>1.25</v>
       </c>
       <c r="F33" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33" s="16">
-        <v>0</v>
+        <f>PRODUCT(F33,Tiers!D3)+F33</f>
+        <v>1.25</v>
       </c>
       <c r="H33" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I33" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L33" s="16">
-        <f>PRODUCT(K33,Tiers!D3)+K33</f>
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,30 +2126,30 @@
         <v>32</v>
       </c>
       <c r="E34" s="17">
-        <f>L34/L32</f>
+        <f>G34/G32</f>
         <v>3</v>
       </c>
       <c r="F34" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34" s="16">
-        <v>0</v>
+        <f>PRODUCT(F34,Tiers!D4)+F34</f>
+        <v>3</v>
       </c>
       <c r="H34" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I34" s="16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J34" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K34" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L34" s="16">
-        <f>PRODUCT(K34,Tiers!D4)+K34</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2163,30 +2166,30 @@
         <v>32</v>
       </c>
       <c r="E35" s="17">
-        <f>L35/L32</f>
+        <f>G35/G32</f>
         <v>6</v>
       </c>
       <c r="F35" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G35" s="16">
-        <v>0</v>
+        <f>PRODUCT(F35,Tiers!D5)+F35</f>
+        <v>6</v>
       </c>
       <c r="H35" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I35" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J35" s="16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K35" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L35" s="16">
-        <f>PRODUCT(K35,Tiers!D5)+K35</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2203,14 +2206,15 @@
         <v>31</v>
       </c>
       <c r="E36" s="17">
-        <f>L36/L32</f>
+        <f>G36/G32</f>
         <v>15</v>
       </c>
-      <c r="F36" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>24</v>
+      <c r="F36" s="16">
+        <v>5</v>
+      </c>
+      <c r="G36" s="16">
+        <f>PRODUCT(F36,Tiers!D6)+F36</f>
+        <v>15</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>24</v>
@@ -2221,12 +2225,11 @@
       <c r="J36" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K36" s="16">
-        <v>5</v>
-      </c>
-      <c r="L36" s="16">
-        <f>PRODUCT(K36,Tiers!D6)+K36</f>
-        <v>15</v>
+      <c r="K36" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implement storage hexes next
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384B1B0B-BD5E-4E47-A4F2-8F3CD1BA81F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A560062E-5B07-4E03-AD42-DE8521BAC168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10365" yWindow="5460" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="140">
   <si>
     <t>Tier</t>
   </si>
@@ -403,22 +403,58 @@
     <t xml:space="preserve">The brain of a creature on the verge of transcending the material plain that was captured and coerced into researching new topics. </t>
   </si>
   <si>
-    <t>A place for basic production and storage of Isolium. Does not require much but in turn does not produce much Isolium.</t>
-  </si>
-  <si>
-    <t>A storehouse where Isolium is produced and stored more efficiently than at a stockpile.</t>
-  </si>
-  <si>
-    <t>A large warehouse for storing and producing Isolium. Due to its size, the warehouse requires more upkeep than a storehouse.</t>
-  </si>
-  <si>
-    <t>A very large complex for producing and storing Isolium. It is also capable of sending the Isolium out more efficently.</t>
-  </si>
-  <si>
     <t>A large, fully automated structure for producing and storing Isolium. Due to its wildly complex structure, it does not lend itself to manual oversight.</t>
   </si>
   <si>
     <t>Here resides the seat of power and the power core keeping the city together. Should it be lost, all will quickly follow so its protection must be prioritized above all else.</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Raw Prod Increases Max Storage Caps for all Resources</t>
+  </si>
+  <si>
+    <t>Isolium Extractor MK I</t>
+  </si>
+  <si>
+    <t>Isolium Extractor MK II</t>
+  </si>
+  <si>
+    <t>Isolium Extractor MK III</t>
+  </si>
+  <si>
+    <t>Isolium Extractor MK IV</t>
+  </si>
+  <si>
+    <t>Isolium Extractor MK V</t>
+  </si>
+  <si>
+    <t>A place for basic production of Isolium. Does not require much but in turn does not produce much Isolium.</t>
+  </si>
+  <si>
+    <t>A large facility for producing Isolium. Due to its size, the MK III requires more upkeep than a MK II.</t>
+  </si>
+  <si>
+    <t>A facility where Isolium is produced more efficiently than a MK I.</t>
+  </si>
+  <si>
+    <t>A very large complex for producing Isolium. It is also capable of sending the Isolium out more efficently.</t>
+  </si>
+  <si>
+    <t>A place where a small amount of items can be stored in a slightly organized pile.</t>
+  </si>
+  <si>
+    <t>A small structure for storing items out of the elements in an organized manner.</t>
+  </si>
+  <si>
+    <t>A large building for storing many items on tall shelves in a very organized manner.</t>
+  </si>
+  <si>
+    <t>A large fully automated building capable of storing many items using complex storage algorithms.</t>
+  </si>
+  <si>
+    <t>An upgraded version of the depot capable of not only receiving items to store but also sending out items before the items were even requested.</t>
   </si>
 </sst>
 </file>
@@ -452,7 +488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +549,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -538,7 +580,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -638,6 +680,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1034,20 +1086,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
-  <dimension ref="A1:AS12"/>
+  <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="20.7109375" style="7" customWidth="1"/>
-    <col min="7" max="45" width="20.7109375" customWidth="1"/>
+    <col min="7" max="41" width="20.7109375" customWidth="1"/>
+    <col min="42" max="42" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20.7109375" customWidth="1"/>
+    <col min="45" max="49" width="20.7109375" style="38" customWidth="1"/>
+    <col min="50" max="50" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -1166,25 +1223,40 @@
         <v>54</v>
       </c>
       <c r="AN1" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO1" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP1" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ1" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR1" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS1" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" s="27" t="s">
+      <c r="AT1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="AP1" s="27" t="s">
+      <c r="AU1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="27" t="s">
+      <c r="AV1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="AR1" s="27" t="s">
+      <c r="AW1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="AS1" s="28" t="s">
+      <c r="AX1" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>71</v>
       </c>
@@ -1317,11 +1389,26 @@
       <c r="AR2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="AS2" s="28" t="s">
+      <c r="AS2" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="AT2" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="AU2" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV2" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW2" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="AX2" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -1454,11 +1541,26 @@
       <c r="AR3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AS3" s="28" t="s">
+      <c r="AS3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU3" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV3" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW3" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="AX3" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>72</v>
       </c>
@@ -1591,11 +1693,26 @@
       <c r="AR4" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AS4" s="28" t="s">
+      <c r="AS4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW4" s="39" t="s">
         <v>28</v>
       </c>
+      <c r="AX4" s="28" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>34</v>
       </c>
@@ -1728,11 +1845,26 @@
       <c r="AR5" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AS5" s="28" t="s">
+      <c r="AS5" s="40">
+        <v>10</v>
+      </c>
+      <c r="AT5" s="40">
+        <v>15</v>
+      </c>
+      <c r="AU5" s="40">
+        <v>25</v>
+      </c>
+      <c r="AV5" s="40">
+        <v>50</v>
+      </c>
+      <c r="AW5" s="40">
+        <v>200</v>
+      </c>
+      <c r="AX5" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>73</v>
       </c>
@@ -1865,11 +1997,26 @@
       <c r="AR6" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AS6" s="28" t="s">
+      <c r="AS6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="40">
+        <v>2</v>
+      </c>
+      <c r="AV6" s="40">
+        <v>3</v>
+      </c>
+      <c r="AW6" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX6" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
@@ -2002,11 +2149,26 @@
       <c r="AR7" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="AS7" s="28" t="s">
+      <c r="AS7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX7" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
@@ -2139,11 +2301,26 @@
       <c r="AR8" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AS8" s="28" t="s">
+      <c r="AS8" s="40">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="40">
+        <v>2</v>
+      </c>
+      <c r="AU8" s="40">
+        <v>3</v>
+      </c>
+      <c r="AV8" s="40">
+        <v>4</v>
+      </c>
+      <c r="AW8" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX8" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -2276,11 +2453,26 @@
       <c r="AR9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AS9" s="28" t="s">
+      <c r="AS9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX9" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -2413,11 +2605,26 @@
       <c r="AR10" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AS10" s="28" t="s">
+      <c r="AS10" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="40">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX10" s="28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>74</v>
       </c>
@@ -2536,25 +2743,40 @@
         <v>121</v>
       </c>
       <c r="AN11" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO11" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AP11" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ11" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR11" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="AO11" s="16" t="s">
+      <c r="AS11" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT11" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU11" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="AV11" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW11" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX11" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="AP11" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="AQ11" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="AR11" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS11" s="17" t="s">
-        <v>127</v>
-      </c>
     </row>
-    <row r="12" spans="1:45" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
@@ -2627,7 +2849,22 @@
       <c r="AP12" s="16"/>
       <c r="AQ12" s="16"/>
       <c r="AR12" s="16"/>
-      <c r="AS12" s="17"/>
+      <c r="AS12" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="AT12" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="AU12" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="AV12" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW12" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX12" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Storage done, power next
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603A5EF0-7A52-46F9-AEE4-C4B243A93A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237C666-4AD5-43B3-B4F1-D1AC6368FE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8280" yWindow="5055" windowWidth="17055" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="152">
   <si>
     <t>Tier</t>
   </si>
@@ -1139,19 +1139,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB11" sqref="BB11"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX5" sqref="AX5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.7109375" style="7" hidden="1" customWidth="1"/>
-    <col min="7" max="41" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="21.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="21.85546875" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="45" max="49" width="20.7109375" style="38" hidden="1" customWidth="1"/>
+    <col min="2" max="6" width="20.7109375" style="7" customWidth="1"/>
+    <col min="7" max="41" width="20.7109375" customWidth="1"/>
+    <col min="42" max="42" width="21.7109375" customWidth="1"/>
+    <col min="43" max="43" width="21.85546875" customWidth="1"/>
+    <col min="44" max="44" width="20.7109375" customWidth="1"/>
+    <col min="45" max="49" width="20.7109375" style="38" customWidth="1"/>
     <col min="50" max="50" width="21.85546875" style="38" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="21.42578125" style="38" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="18.5703125" style="38" bestFit="1" customWidth="1"/>
@@ -1822,7 +1822,7 @@
         <v>29</v>
       </c>
       <c r="BB4" s="42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BC4" s="28" t="s">
         <v>28</v>
@@ -2155,8 +2155,8 @@
       <c r="BA6" s="43">
         <v>3</v>
       </c>
-      <c r="BB6" s="43" t="s">
-        <v>22</v>
+      <c r="BB6" s="43">
+        <v>5</v>
       </c>
       <c r="BC6" s="28" t="s">
         <v>22</v>
@@ -2322,8 +2322,8 @@
       <c r="BA7" s="43">
         <v>0</v>
       </c>
-      <c r="BB7" s="43" t="s">
-        <v>22</v>
+      <c r="BB7" s="43">
+        <v>0</v>
       </c>
       <c r="BC7" s="28" t="s">
         <v>22</v>
@@ -2489,8 +2489,8 @@
       <c r="BA8" s="43">
         <v>4</v>
       </c>
-      <c r="BB8" s="43" t="s">
-        <v>22</v>
+      <c r="BB8" s="43">
+        <v>5</v>
       </c>
       <c r="BC8" s="28" t="s">
         <v>22</v>
@@ -2656,8 +2656,8 @@
       <c r="BA9" s="43">
         <v>0</v>
       </c>
-      <c r="BB9" s="43" t="s">
-        <v>22</v>
+      <c r="BB9" s="43">
+        <v>0</v>
       </c>
       <c r="BC9" s="28" t="s">
         <v>22</v>
@@ -2823,8 +2823,8 @@
       <c r="BA10" s="43">
         <v>0</v>
       </c>
-      <c r="BB10" s="43" t="s">
-        <v>22</v>
+      <c r="BB10" s="43">
+        <v>0</v>
       </c>
       <c r="BC10" s="28" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
Entertainment, specialty buildings, and research next
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237C666-4AD5-43B3-B4F1-D1AC6368FE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B8260-DACD-4FE2-9772-912DCAE61FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
     <sheet name="Buildings" sheetId="3" r:id="rId2"/>
+    <sheet name="Specialty Buildings" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="207">
   <si>
     <t>Tier</t>
   </si>
@@ -491,6 +492,171 @@
   </si>
   <si>
     <t>A power plant perfected by harvesting power from alternate dimensions where power flows freely or not. No one is really sure how or even why it works, though it is best not to question it.</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Public Park</t>
+  </si>
+  <si>
+    <t>Theater Complex</t>
+  </si>
+  <si>
+    <t>Circus</t>
+  </si>
+  <si>
+    <t>Virtual Reality Café</t>
+  </si>
+  <si>
+    <t>A simple grassy field open for anyone to use for various outdoor activities.</t>
+  </si>
+  <si>
+    <t>A traveling circus that entertains guests with fantastical performances without travelling.</t>
+  </si>
+  <si>
+    <t>A group of theaters that show everything from student performances to blockbuster superhero movies. Fans of both believe their perference is better than the other.</t>
+  </si>
+  <si>
+    <t>A gathering spot that rents VR headsets to customers for entertainment or simply to forget how lonely they are.</t>
+  </si>
+  <si>
+    <t>Quantum Hologram Theater</t>
+  </si>
+  <si>
+    <t>A theater that uses holograms and quantum technology to insert the viewer directly into the experience. Barf bags are not included.</t>
+  </si>
+  <si>
+    <t>Void Portal</t>
+  </si>
+  <si>
+    <t>Void Communicator</t>
+  </si>
+  <si>
+    <t>Void Radar Array</t>
+  </si>
+  <si>
+    <t>Faction Embassy</t>
+  </si>
+  <si>
+    <t>Weather Manipulator</t>
+  </si>
+  <si>
+    <t>Abyssal Pathfinder</t>
+  </si>
+  <si>
+    <t>Void Rudder</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Unlocks direct travel to other factions including raiding and defending allies</t>
+  </si>
+  <si>
+    <t>Unlocks communication with other factions for trading, diplomacy, and requests</t>
+  </si>
+  <si>
+    <t>Passively builds up charge and on discharge discovers a new point of interest(factions, events, etc) in the Void</t>
+  </si>
+  <si>
+    <t>Generic embassy for a given faction and prevents reputation degredation. On destruction, reputation will take a massive hit causing the faction to cut ties or at worst attack the player</t>
+  </si>
+  <si>
+    <t>Allows for the traversal of the Abyss but takes a long time to find a vaiable path.</t>
+  </si>
+  <si>
+    <t>Required for Win State</t>
+  </si>
+  <si>
+    <t>Military, Diplomacy</t>
+  </si>
+  <si>
+    <t>Military, Diplomacy, Tech</t>
+  </si>
+  <si>
+    <t>Diplomacy</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Very slowly moves the player's Sanctuary closer to the Abyss. More increase the speed the Sanctuary is moved.</t>
+  </si>
+  <si>
+    <t>Prod adds to happiness for each house in area. Effect decreases by 10 each hex distance away from self</t>
+  </si>
+  <si>
+    <t>Allows the player to change the weather of their Sanctuary for an isolium cost. Selecting the population requested weather provides a large happiness bonus to all houses</t>
+  </si>
+  <si>
+    <t>A large circular structure that utilizes the inherently volatile energies of the void to create a semi-stable wormhole between two points. Due to the massive amount of energy channeled by the device, its destruction is not recommended and its operation tends to send shockwaves across the Sanctuary.</t>
+  </si>
+  <si>
+    <t>A communications array that utilizes quantum technologies to send messages to the where the recipient was and will be simaltainously. No one is truly sure how or even why it works except that asking would probably break it.</t>
+  </si>
+  <si>
+    <t>A large array of radar dishes that scans for disturbances in the Void to find anomalies. Once an anomaly is found however, the radar array's job is done and the anomaly must be scouted.</t>
+  </si>
+  <si>
+    <t>An embassy to [FACTION] for both sides to maintain friendly relations. Prevents reputation degredation but will cause significant damage if destroyed.</t>
+  </si>
+  <si>
+    <t>A large supercomputer capable of calculating a safe path through the Abyss. However due to the complexity of the Abyss, it takes a long time to find a viable path.</t>
+  </si>
+  <si>
+    <t>While the initial idea of strapping massive engines to the Sanctuary to move sounded ludicrous, the final version is very reasonable and somewhat practical. Building more Void Rudders will increase the speed the Sanctuary is moved at.</t>
+  </si>
+  <si>
+    <t>A large device capable of changing the weather manipulating the Void at the edges of the Sanctuary. Providing the requested weather will provide a large happiness bonus to the entire Sanctuary.</t>
+  </si>
+  <si>
+    <t>Randomized Desc, Randomized Building/Art, Ramping Cost, Less Ramping Bonuses</t>
+  </si>
+  <si>
+    <t>Diplomatic Monument</t>
+  </si>
+  <si>
+    <t>Scientific Monument</t>
+  </si>
+  <si>
+    <t>Happiness Monument</t>
+  </si>
+  <si>
+    <t>Industry Monument</t>
+  </si>
+  <si>
+    <t>Isolium Monument</t>
+  </si>
+  <si>
+    <t>Military Monument</t>
+  </si>
+  <si>
+    <t>Food Monument</t>
+  </si>
+  <si>
+    <t>+ Research Speed</t>
+  </si>
+  <si>
+    <t>+ Sanctuary Happiness</t>
+  </si>
+  <si>
+    <t>+ Industry Prod</t>
+  </si>
+  <si>
+    <t>+ Isolium Prod</t>
+  </si>
+  <si>
+    <t>+ Combat Unit Stats</t>
+  </si>
+  <si>
+    <t>+ Food Prod</t>
+  </si>
+  <si>
+    <t>+ Diplomatic Action Cost Reduc</t>
   </si>
 </sst>
 </file>
@@ -500,7 +666,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,8 +689,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,6 +769,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF79E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -622,7 +800,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -742,6 +920,19 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -753,6 +944,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF79E5"/>
       <color rgb="FF960000"/>
       <color rgb="FFA162D0"/>
       <color rgb="FFFFD700"/>
@@ -1137,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
-  <dimension ref="A1:BC12"/>
+  <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX5" sqref="AX5"/>
+    <sheetView topLeftCell="BA1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BK11" sqref="BK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -1152,15 +1344,17 @@
     <col min="43" max="43" width="21.85546875" customWidth="1"/>
     <col min="44" max="44" width="20.7109375" customWidth="1"/>
     <col min="45" max="49" width="20.7109375" style="38" customWidth="1"/>
-    <col min="50" max="50" width="21.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="21.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="18.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.85546875" style="38" customWidth="1"/>
+    <col min="51" max="51" width="21.42578125" style="38" customWidth="1"/>
+    <col min="52" max="52" width="18.5703125" style="38" customWidth="1"/>
+    <col min="53" max="53" width="19.28515625" style="38" customWidth="1"/>
     <col min="54" max="54" width="20.7109375" style="38" customWidth="1"/>
-    <col min="55" max="55" width="20.7109375" customWidth="1"/>
+    <col min="55" max="58" width="20.7109375" customWidth="1"/>
+    <col min="59" max="59" width="26.140625" customWidth="1"/>
+    <col min="60" max="60" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -1323,11 +1517,26 @@
       <c r="BB1" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="BC1" s="28" t="s">
+      <c r="BC1" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="BD1" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE1" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="BF1" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="BG1" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="BH1" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>71</v>
       </c>
@@ -1490,11 +1699,26 @@
       <c r="BB2" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="BC2" s="28" t="s">
+      <c r="BC2" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD2" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE2" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="BF2" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="BG2" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="BH2" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -1657,11 +1881,26 @@
       <c r="BB3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="BC3" s="28" t="s">
+      <c r="BC3" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD3" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE3" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF3" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG3" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH3" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>72</v>
       </c>
@@ -1824,11 +2063,26 @@
       <c r="BB4" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="BC4" s="28" t="s">
+      <c r="BC4" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD4" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="BE4" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF4" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG4" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="BH4" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>34</v>
       </c>
@@ -1991,11 +2245,26 @@
       <c r="BB5" s="43">
         <v>5</v>
       </c>
-      <c r="BC5" s="28" t="s">
+      <c r="BC5" s="47">
+        <v>10</v>
+      </c>
+      <c r="BD5" s="47">
+        <v>20</v>
+      </c>
+      <c r="BE5" s="47">
+        <v>30</v>
+      </c>
+      <c r="BF5" s="47">
+        <v>40</v>
+      </c>
+      <c r="BG5" s="47">
+        <v>50</v>
+      </c>
+      <c r="BH5" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>73</v>
       </c>
@@ -2158,11 +2427,26 @@
       <c r="BB6" s="43">
         <v>5</v>
       </c>
-      <c r="BC6" s="28" t="s">
+      <c r="BC6" s="47">
+        <v>1</v>
+      </c>
+      <c r="BD6" s="47">
+        <v>2</v>
+      </c>
+      <c r="BE6" s="47">
+        <v>1</v>
+      </c>
+      <c r="BF6" s="47">
+        <v>1</v>
+      </c>
+      <c r="BG6" s="47">
+        <v>3</v>
+      </c>
+      <c r="BH6" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
@@ -2325,11 +2609,26 @@
       <c r="BB7" s="43">
         <v>0</v>
       </c>
-      <c r="BC7" s="28" t="s">
+      <c r="BC7" s="47">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="47">
+        <v>2</v>
+      </c>
+      <c r="BE7" s="47">
+        <v>3</v>
+      </c>
+      <c r="BF7" s="47">
+        <v>2</v>
+      </c>
+      <c r="BG7" s="47">
+        <v>3</v>
+      </c>
+      <c r="BH7" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
@@ -2492,11 +2791,26 @@
       <c r="BB8" s="43">
         <v>5</v>
       </c>
-      <c r="BC8" s="28" t="s">
+      <c r="BC8" s="47">
+        <v>1</v>
+      </c>
+      <c r="BD8" s="47">
+        <v>1</v>
+      </c>
+      <c r="BE8" s="47">
+        <v>3</v>
+      </c>
+      <c r="BF8" s="47">
+        <v>4</v>
+      </c>
+      <c r="BG8" s="47">
+        <v>5</v>
+      </c>
+      <c r="BH8" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -2659,11 +2973,26 @@
       <c r="BB9" s="43">
         <v>0</v>
       </c>
-      <c r="BC9" s="28" t="s">
+      <c r="BC9" s="47">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="47">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="47">
+        <v>1</v>
+      </c>
+      <c r="BF9" s="47">
+        <v>3</v>
+      </c>
+      <c r="BG9" s="47">
+        <v>5</v>
+      </c>
+      <c r="BH9" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:55" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -2826,11 +3155,26 @@
       <c r="BB10" s="43">
         <v>0</v>
       </c>
-      <c r="BC10" s="28" t="s">
+      <c r="BC10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:55" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>74</v>
       </c>
@@ -2993,11 +3337,26 @@
       <c r="BB11" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="BC11" s="17" t="s">
+      <c r="BC11" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="BD11" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE11" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="BF11" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="BG11" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="BH11" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:55" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:60" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
@@ -3100,10 +3459,642 @@
       <c r="BB12" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="BC12" s="17"/>
+      <c r="BC12" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD12" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="BE12" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="BF12" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="BG12" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="BH12" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833B062E-FF43-4862-99AD-38C3925F7752}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" t="s">
+        <v>195</v>
+      </c>
+      <c r="L1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N2" t="s">
+        <v>170</v>
+      </c>
+      <c r="O2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M5" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="N5" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="O5" s="49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>15</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>15</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>20</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>20</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="45" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="45" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="I12" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="J12" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="L12" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="M12" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="N12" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="O12" s="45" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" t="s">
+        <v>180</v>
+      </c>
+      <c r="H13" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" t="s">
+        <v>181</v>
+      </c>
+      <c r="J13" t="s">
+        <v>181</v>
+      </c>
+      <c r="K13" t="s">
+        <v>181</v>
+      </c>
+      <c r="L13" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" t="s">
+        <v>181</v>
+      </c>
+      <c r="N13" t="s">
+        <v>181</v>
+      </c>
+      <c r="O13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
entertainment progress.  Pop growth next
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B8260-DACD-4FE2-9772-912DCAE61FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D54416-844A-4057-9A89-1D18FB4368C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4365" windowWidth="17055" windowHeight="6435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="207">
   <si>
     <t>Tier</t>
   </si>
@@ -1331,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView topLeftCell="BA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BK11" sqref="BK11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:BC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -2076,7 +2076,7 @@
         <v>29</v>
       </c>
       <c r="BG4" s="47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BH4" s="28" t="s">
         <v>28</v>
@@ -2439,8 +2439,8 @@
       <c r="BF6" s="47">
         <v>1</v>
       </c>
-      <c r="BG6" s="47">
-        <v>3</v>
+      <c r="BG6" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="BH6" s="28" t="s">
         <v>22</v>
@@ -2621,8 +2621,8 @@
       <c r="BF7" s="47">
         <v>2</v>
       </c>
-      <c r="BG7" s="47">
-        <v>3</v>
+      <c r="BG7" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="BH7" s="28" t="s">
         <v>22</v>
@@ -2803,8 +2803,8 @@
       <c r="BF8" s="47">
         <v>4</v>
       </c>
-      <c r="BG8" s="47">
-        <v>5</v>
+      <c r="BG8" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="BH8" s="28" t="s">
         <v>22</v>
@@ -2985,8 +2985,8 @@
       <c r="BF9" s="47">
         <v>3</v>
       </c>
-      <c r="BG9" s="47">
-        <v>5</v>
+      <c r="BG9" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="BH9" s="28" t="s">
         <v>22</v>
@@ -3167,8 +3167,8 @@
       <c r="BF10" s="47">
         <v>0</v>
       </c>
-      <c r="BG10" s="47">
-        <v>0</v>
+      <c r="BG10" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="BH10" s="28" t="s">
         <v>83</v>
@@ -3486,8 +3486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833B062E-FF43-4862-99AD-38C3925F7752}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,10 +3495,10 @@
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="29.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="20.28515625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
New building shells in, focus on Implementation next
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D54416-844A-4057-9A89-1D18FB4368C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D620258-A5EB-499D-98D2-BF8A75D35DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4365" windowWidth="17055" windowHeight="6435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -1331,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:BC1048576"/>
     </sheetView>
   </sheetViews>
@@ -3486,8 +3486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833B062E-FF43-4862-99AD-38C3925F7752}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3517,13 +3517,13 @@
         <v>165</v>
       </c>
       <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" t="s">
         <v>166</v>
-      </c>
-      <c r="F1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G1" t="s">
-        <v>169</v>
       </c>
       <c r="H1" t="s">
         <v>167</v>
@@ -3752,13 +3752,13 @@
         <v>5</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>10</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3799,13 +3799,13 @@
         <v>0</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>10</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3846,13 +3846,13 @@
         <v>50</v>
       </c>
       <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
         <v>5</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>50</v>
       </c>
       <c r="H8">
         <v>50</v>
@@ -3893,13 +3893,13 @@
         <v>50</v>
       </c>
       <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
         <v>5</v>
-      </c>
-      <c r="F9">
-        <v>100</v>
-      </c>
-      <c r="G9">
-        <v>50</v>
       </c>
       <c r="H9">
         <v>50</v>
@@ -3940,13 +3940,13 @@
         <v>0</v>
       </c>
       <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>5</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -3987,13 +3987,13 @@
         <v>187</v>
       </c>
       <c r="E11" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G11" s="45" t="s">
         <v>188</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>190</v>
       </c>
       <c r="H11" s="45" t="s">
         <v>191</v>
@@ -4013,13 +4013,13 @@
         <v>173</v>
       </c>
       <c r="E12" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="45" t="s">
         <v>174</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="G12" s="45" t="s">
-        <v>182</v>
       </c>
       <c r="H12" s="45" t="s">
         <v>184</v>
@@ -4060,13 +4060,13 @@
         <v>178</v>
       </c>
       <c r="E13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F13" t="s">
         <v>180</v>
       </c>
       <c r="G13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H13" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
bug fixes and UI tweaks again
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D620258-A5EB-499D-98D2-BF8A75D35DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A526DEB-5133-4D0E-A8EB-260853835B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="214">
   <si>
     <t>Tier</t>
   </si>
@@ -657,6 +657,27 @@
   </si>
   <si>
     <t>+ Diplomatic Action Cost Reduc</t>
+  </si>
+  <si>
+    <t>IMPLEMENTATION STATUS</t>
+  </si>
+  <si>
+    <t>Implementation Status</t>
+  </si>
+  <si>
+    <t>NOT STARTED</t>
+  </si>
+  <si>
+    <t>SHELL</t>
+  </si>
+  <si>
+    <t>STARTED</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>FINISHED</t>
   </si>
 </sst>
 </file>
@@ -800,7 +821,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -933,6 +954,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -940,7 +965,78 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1224,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,9 +1331,10 @@
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,8 +1347,11 @@
       <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="G1" s="50" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1264,8 +1364,11 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
+      <c r="G2" t="s">
+        <v>209</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1278,8 +1381,11 @@
       <c r="D3" s="5">
         <v>0.25</v>
       </c>
+      <c r="G3" t="s">
+        <v>210</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1292,8 +1398,11 @@
       <c r="D4" s="5">
         <v>0.5</v>
       </c>
+      <c r="G4" t="s">
+        <v>211</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1306,8 +1415,11 @@
       <c r="D5" s="5">
         <v>1</v>
       </c>
+      <c r="G5" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1319,6 +1431,9 @@
       </c>
       <c r="D6" s="5">
         <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1329,15 +1444,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
-  <dimension ref="A1:BH12"/>
+  <dimension ref="A1:BH13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:BC1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="6" customWidth="1"/>
     <col min="2" max="6" width="20.7109375" style="7" customWidth="1"/>
     <col min="7" max="41" width="20.7109375" customWidth="1"/>
     <col min="42" max="42" width="21.7109375" customWidth="1"/>
@@ -3476,23 +3591,279 @@
       </c>
       <c r="BH12" s="17"/>
     </row>
+    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="L13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="M13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="O13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="P13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="R13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="S13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="T13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="U13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="V13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="W13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="X13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AE13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AI13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AM13" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="AN13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AO13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AP13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AQ13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AR13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AS13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AV13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AW13" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="AX13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BA13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BB13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BC13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BD13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BF13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BG13" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="BH13" s="51" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{98ED36B8-A279-4C77-AB57-9EC7D24FFB6C}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$2,B13)))</xm:f>
+            <xm:f>Tiers!$G$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC00000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{4F6E6EB3-A34A-46BD-8A7F-3E1A26A40259}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$3,B13)))</xm:f>
+            <xm:f>Tiers!$G$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{AA3967A1-817B-49EE-83E4-0FA5B7771630}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$4,B13)))</xm:f>
+            <xm:f>Tiers!$G$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{73223FEE-7109-41FD-83AD-7C62F00EA6E5}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$5,B13)))</xm:f>
+            <xm:f>Tiers!$G$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{6740D5E2-EAC6-40B3-BF7B-A102C82DBF29}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$6,B13)))</xm:f>
+            <xm:f>Tiers!$G$6</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B13:BH13</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1EF31FA6-0B72-4669-89A0-DF93CF264664}">
+          <x14:formula1>
+            <xm:f>Tiers!$G$2:$G$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13:BH13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833B062E-FF43-4862-99AD-38C3925F7752}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:BH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="29.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
@@ -3503,7 +3874,7 @@
     <col min="15" max="15" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3550,7 +3921,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>71</v>
       </c>
@@ -3597,7 +3968,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -3644,7 +4015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>72</v>
       </c>
@@ -3691,7 +4062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>34</v>
       </c>
@@ -3738,7 +4109,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>73</v>
       </c>
@@ -3785,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
@@ -3832,7 +4203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
@@ -3879,7 +4250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -3926,7 +4297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -3973,7 +4344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="45" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" s="45" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>74</v>
       </c>
@@ -3999,7 +4370,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="45" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:60" s="45" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
@@ -4046,7 +4417,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>176</v>
       </c>
@@ -4092,9 +4463,175 @@
       <c r="O13" t="s">
         <v>181</v>
       </c>
+    </row>
+    <row r="14" spans="1:60" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="H14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="I14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="K14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="L14" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="M14" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="N14" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="O14" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="51"/>
+      <c r="AI14" s="51"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="51"/>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="51"/>
+      <c r="AP14" s="51"/>
+      <c r="AQ14" s="51"/>
+      <c r="AR14" s="51"/>
+      <c r="AS14" s="51"/>
+      <c r="AT14" s="51"/>
+      <c r="AU14" s="51"/>
+      <c r="AV14" s="51"/>
+      <c r="AW14" s="51"/>
+      <c r="AX14" s="51"/>
+      <c r="AY14" s="51"/>
+      <c r="AZ14" s="51"/>
+      <c r="BA14" s="51"/>
+      <c r="BB14" s="51"/>
+      <c r="BC14" s="51"/>
+      <c r="BD14" s="51"/>
+      <c r="BE14" s="51"/>
+      <c r="BF14" s="51"/>
+      <c r="BG14" s="51"/>
+      <c r="BH14" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{ACC789E1-FE5F-4456-A5C8-9F2C1BE04049}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$6,B14)))</xm:f>
+            <xm:f>Tiers!$G$6</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{25133FF0-E929-4020-8D53-245B6DF69F88}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$5,B14)))</xm:f>
+            <xm:f>Tiers!$G$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{6E0C9BD1-D8C2-4C5D-AFBC-24C38CEED168}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$4,B14)))</xm:f>
+            <xm:f>Tiers!$G$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{5FEF1AB5-D211-44B9-A883-CD8DC62717E3}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$3,B14)))</xm:f>
+            <xm:f>Tiers!$G$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{10455162-ED76-4B3D-8C86-31C09D66E6EA}">
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$2,B14)))</xm:f>
+            <xm:f>Tiers!$G$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC00000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B14:O14</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{2DDEC59F-E6EF-4328-B82C-C9A798B9075A}">
+          <x14:formula1>
+            <xm:f>Tiers!$G$2:$G$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B14:O14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upkeep integration and resource prod overhaul
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F65ECD-DCDA-468A-8E5C-37DEAA598947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3255F70-1386-4256-90AC-18C1DFDFCE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="252">
   <si>
     <t>Tier</t>
   </si>
@@ -686,9 +686,6 @@
     <t>Monument</t>
   </si>
   <si>
-    <t>Upkeep Per Tick</t>
-  </si>
-  <si>
     <t>1 FOOD + 1.5 IND + 1.5 ISO</t>
   </si>
   <si>
@@ -726,6 +723,75 @@
   </si>
   <si>
     <t>0.5 FOOD + 2 IND</t>
+  </si>
+  <si>
+    <t>Tick Rates</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Upkeep</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>1 per second</t>
+  </si>
+  <si>
+    <t>1 per minute</t>
+  </si>
+  <si>
+    <t>Upkeep Per Second</t>
+  </si>
+  <si>
+    <t>Production Per Second</t>
+  </si>
+  <si>
+    <t>Production Per Minute</t>
+  </si>
+  <si>
+    <t>Upkeep Per Minute</t>
+  </si>
+  <si>
+    <t>90 FOOD + 120 IND + 120 ISO</t>
+  </si>
+  <si>
+    <t>45 FOOD + 60 IND + 60 ISO</t>
+  </si>
+  <si>
+    <t>60 FOOD + 90 IND + 90 ISO</t>
+  </si>
+  <si>
+    <t>120 FOOD + 180 IND + 180 ISO</t>
+  </si>
+  <si>
+    <t>30 FOOD + 30 IND + 30 ISO</t>
+  </si>
+  <si>
+    <t>60 FOOD + 60 IND + 60 ISO</t>
+  </si>
+  <si>
+    <t>90 FOOD + 90 IND + 90 ISO</t>
+  </si>
+  <si>
+    <t>120 IND + 120 ISO</t>
+  </si>
+  <si>
+    <t>150 IND + 150 ISO</t>
+  </si>
+  <si>
+    <t>30 FOOD + 30 IND</t>
+  </si>
+  <si>
+    <t>60 FOOD + 30 IND</t>
+  </si>
+  <si>
+    <t>30 FOOD + 90 IND</t>
+  </si>
+  <si>
+    <t>30 FOOD + 120 IND</t>
   </si>
 </sst>
 </file>
@@ -869,7 +935,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1038,6 +1104,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -1120,8 +1192,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF960000"/>
       <color rgb="FFFF79E5"/>
-      <color rgb="FF960000"/>
       <color rgb="FFA162D0"/>
       <color rgb="FFFFD700"/>
     </mruColors>
@@ -1400,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,11 +1483,13 @@
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1428,14 +1502,20 @@
       <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1448,14 +1528,20 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>209</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="J2" t="s">
+        <v>230</v>
+      </c>
+      <c r="K2" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1468,14 +1554,20 @@
       <c r="D3" s="5">
         <v>0.25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>210</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
+      <c r="J3" t="s">
+        <v>231</v>
+      </c>
+      <c r="K3" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1488,14 +1580,14 @@
       <c r="D4" s="5">
         <v>0.5</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>211</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1508,14 +1600,14 @@
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>212</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1528,50 +1620,50 @@
       <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>213</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
         <v>215</v>
       </c>
     </row>
@@ -1583,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
-  <dimension ref="A1:BH14"/>
+  <dimension ref="A1:BI17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BG14" sqref="BG14"/>
+      <selection activeCell="BI12" sqref="BI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -1608,7 +1700,7 @@
     <col min="60" max="60" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -1790,7 +1882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>71</v>
       </c>
@@ -1972,7 +2064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>72</v>
       </c>
@@ -2336,7 +2428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>34</v>
       </c>
@@ -2466,8 +2558,8 @@
       <c r="AQ5" s="37">
         <v>4</v>
       </c>
-      <c r="AR5" s="37" t="s">
-        <v>81</v>
+      <c r="AR5" s="37">
+        <v>5</v>
       </c>
       <c r="AS5" s="40">
         <v>10</v>
@@ -2518,7 +2610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>73</v>
       </c>
@@ -2700,7 +2792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
@@ -2882,7 +2974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
@@ -3064,7 +3156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -3246,7 +3338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:60" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -3428,689 +3520,1331 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:60" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
-        <v>216</v>
-      </c>
-      <c r="B11" s="52" t="str">
+    <row r="11" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="31">
+        <f>B5</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="31">
+        <f>C5</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="31">
+        <f>D5</f>
+        <v>3</v>
+      </c>
+      <c r="E11" s="31">
+        <f>E5</f>
+        <v>4</v>
+      </c>
+      <c r="F11" s="31">
+        <f>F5</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="32">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="32">
+        <f>H5</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="32">
+        <f>I5</f>
+        <v>3</v>
+      </c>
+      <c r="J11" s="32">
+        <f>J5</f>
+        <v>4</v>
+      </c>
+      <c r="K11" s="32">
+        <f>K5</f>
+        <v>5</v>
+      </c>
+      <c r="L11" s="33">
+        <f>L5</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="33">
+        <f>M5</f>
+        <v>2</v>
+      </c>
+      <c r="N11" s="33">
+        <f>N5</f>
+        <v>3</v>
+      </c>
+      <c r="O11" s="33">
+        <f>O5</f>
+        <v>4</v>
+      </c>
+      <c r="P11" s="33">
+        <f>P5</f>
+        <v>5</v>
+      </c>
+      <c r="Q11" s="34">
+        <f>Q5</f>
+        <v>1</v>
+      </c>
+      <c r="R11" s="34">
+        <f>R5</f>
+        <v>2</v>
+      </c>
+      <c r="S11" s="34">
+        <f>S5</f>
+        <v>3</v>
+      </c>
+      <c r="T11" s="34">
+        <f>T5</f>
+        <v>4</v>
+      </c>
+      <c r="U11" s="34">
+        <f>U5</f>
+        <v>5</v>
+      </c>
+      <c r="V11" s="35" t="str">
+        <f>V5</f>
+        <v>NULL</v>
+      </c>
+      <c r="W11" s="35" t="str">
+        <f>W5</f>
+        <v>NULL</v>
+      </c>
+      <c r="X11" s="35" t="str">
+        <f>X5</f>
+        <v>NULL</v>
+      </c>
+      <c r="Y11" s="35" t="str">
+        <f>Y5</f>
+        <v>NULL</v>
+      </c>
+      <c r="Z11" s="35" t="str">
+        <f>Z5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AA11" s="35" t="str">
+        <f>AA5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AB11" s="35" t="str">
+        <f>AB5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AC11" s="35" t="str">
+        <f>AC5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AD11" s="30" t="str">
+        <f>AD5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AE11" s="30" t="str">
+        <f>AE5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AF11" s="30" t="str">
+        <f>AF5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AG11" s="30" t="str">
+        <f>AG5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AH11" s="30" t="str">
+        <f>AH5</f>
+        <v>NULL</v>
+      </c>
+      <c r="AI11" s="36">
+        <f>AI5</f>
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="36">
+        <f>AJ5</f>
+        <v>2</v>
+      </c>
+      <c r="AK11" s="36">
+        <f>AK5</f>
+        <v>3</v>
+      </c>
+      <c r="AL11" s="36">
+        <f>AL5</f>
+        <v>4</v>
+      </c>
+      <c r="AM11" s="36">
+        <f>AM5</f>
+        <v>5</v>
+      </c>
+      <c r="AN11" s="37">
+        <f>AN5</f>
+        <v>1</v>
+      </c>
+      <c r="AO11" s="37">
+        <f>AO5</f>
+        <v>2</v>
+      </c>
+      <c r="AP11" s="37">
+        <f>AP5</f>
+        <v>3</v>
+      </c>
+      <c r="AQ11" s="37">
+        <f>AQ5</f>
+        <v>4</v>
+      </c>
+      <c r="AR11" s="37">
+        <f>AR5</f>
+        <v>5</v>
+      </c>
+      <c r="AS11" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT11" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU11" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV11" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW11" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX11" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY11" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ11" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA11" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB11" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC11" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD11" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE11" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF11" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BG11" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH11" s="62" t="str">
+        <f>BH5</f>
+        <v>NULL</v>
+      </c>
+      <c r="BI11" s="50"/>
+    </row>
+    <row r="12" spans="1:61" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A12" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="52" t="str">
         <f>B5 * 0.5 &amp;" IND + " &amp; B5 * 0.5 &amp; " ISO"</f>
         <v>0.5 IND + 0.5 ISO</v>
       </c>
-      <c r="C11" s="52" t="str">
+      <c r="C12" s="52" t="str">
         <f>C5 * 0.5 &amp;" IND + " &amp; C5 * 0.5 &amp; " ISO"</f>
         <v>1 IND + 1 ISO</v>
       </c>
-      <c r="D11" s="52" t="str">
+      <c r="D12" s="52" t="str">
         <f>D5 * 0.5 &amp;" IND + " &amp; D5 * 0.5 &amp; " ISO"</f>
         <v>1.5 IND + 1.5 ISO</v>
       </c>
-      <c r="E11" s="52" t="str">
+      <c r="E12" s="52" t="str">
         <f>E5 * 0.5 &amp;" IND + " &amp; E5 * 0.5 &amp; " ISO"</f>
         <v>2 IND + 2 ISO</v>
       </c>
-      <c r="F11" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="53" t="str">
+      <c r="F12" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="53" t="str">
         <f>G5 * 0.75 &amp;" FOOD"</f>
         <v>0.75 FOOD</v>
       </c>
-      <c r="H11" s="53" t="str">
+      <c r="H12" s="53" t="str">
         <f>H5 * 0.75 &amp;" FOOD"</f>
         <v>1.5 FOOD</v>
       </c>
-      <c r="I11" s="53" t="str">
+      <c r="I12" s="53" t="str">
         <f>I5 * 0.75 &amp;" FOOD"</f>
         <v>2.25 FOOD</v>
       </c>
-      <c r="J11" s="53" t="str">
+      <c r="J12" s="53" t="str">
         <f>J5 * 0.75 &amp;" FOOD"</f>
         <v>3 FOOD</v>
       </c>
-      <c r="K11" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="54" t="str">
+      <c r="K12" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="54" t="str">
         <f>L5 * 0.75 &amp;" ISO"</f>
         <v>0.75 ISO</v>
       </c>
-      <c r="M11" s="54" t="str">
+      <c r="M12" s="54" t="str">
         <f>M5 * 0.75 &amp;" ISO"</f>
         <v>1.5 ISO</v>
       </c>
-      <c r="N11" s="54" t="str">
+      <c r="N12" s="54" t="str">
         <f>N5 * 0.75 &amp;" ISO"</f>
         <v>2.25 ISO</v>
       </c>
-      <c r="O11" s="54" t="str">
+      <c r="O12" s="54" t="str">
         <f>O5 * 0.75 &amp;" ISO"</f>
         <v>3 ISO</v>
       </c>
-      <c r="P11" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q11" s="55" t="str">
+      <c r="P12" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="55" t="str">
         <f>Q5 * 0.5 &amp;" FOOD + " &amp;Q5 * 0.75 &amp;" IND + "&amp;Q5 * 0.75&amp;" ISO"</f>
         <v>0.5 FOOD + 0.75 IND + 0.75 ISO</v>
       </c>
-      <c r="R11" s="55" t="str">
+      <c r="R12" s="55" t="str">
         <f>R5 * 0.5 &amp;" FOOD + " &amp;R5 * 0.75 &amp;" IND + "&amp;R5 * 0.75&amp;" ISO"</f>
         <v>1 FOOD + 1.5 IND + 1.5 ISO</v>
       </c>
-      <c r="S11" s="55" t="str">
+      <c r="S12" s="55" t="str">
         <f>S5 * 0.5 &amp;" FOOD + " &amp;S5 * 0.75 &amp;" IND + "&amp;S5 * 0.75&amp;" ISO"</f>
         <v>1.5 FOOD + 2.25 IND + 2.25 ISO</v>
       </c>
-      <c r="T11" s="55" t="str">
+      <c r="T12" s="55" t="str">
         <f>T5 * 0.5 &amp;" FOOD + " &amp;T5 * 0.75 &amp;" IND + "&amp;T5 * 0.75&amp;" ISO"</f>
         <v>2 FOOD + 3 IND + 3 ISO</v>
       </c>
-      <c r="U11" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="V11" s="56" t="s">
+      <c r="U12" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="W12" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="X12" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y12" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="W11" s="56" t="s">
-        <v>217</v>
-      </c>
-      <c r="X11" s="56" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y11" s="56" t="s">
+      <c r="Z12" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA12" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="Z11" s="56" t="s">
+      <c r="AB12" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="AA11" s="56" t="s">
+      <c r="AC12" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD12" s="57" t="s">
         <v>220</v>
       </c>
-      <c r="AB11" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="AC11" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="AD11" s="57" t="s">
+      <c r="AE12" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="AE11" s="57" t="s">
+      <c r="AF12" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="AF11" s="57" t="s">
+      <c r="AG12" s="57" t="s">
         <v>223</v>
       </c>
-      <c r="AG11" s="57" t="s">
+      <c r="AH12" s="57" t="s">
         <v>224</v>
       </c>
-      <c r="AH11" s="57" t="s">
-        <v>225</v>
-      </c>
-      <c r="AI11" s="58" t="str">
+      <c r="AI12" s="58" t="str">
         <f>AI5 *0.5&amp;" ISO"</f>
         <v>0.5 ISO</v>
       </c>
-      <c r="AJ11" s="58" t="str">
+      <c r="AJ12" s="58" t="str">
         <f>AJ5 *0.5&amp;" ISO"</f>
         <v>1 ISO</v>
       </c>
-      <c r="AK11" s="58" t="str">
+      <c r="AK12" s="58" t="str">
         <f>AK5 *0.5&amp;" ISO"</f>
         <v>1.5 ISO</v>
       </c>
-      <c r="AL11" s="58" t="str">
+      <c r="AL12" s="58" t="str">
         <f>AL5 *0.5&amp;" ISO"</f>
         <v>2 ISO</v>
       </c>
-      <c r="AM11" s="58" t="s">
+      <c r="AM12" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="AN11" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO11" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP11" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="AQ11" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR11" s="59" t="s">
+      <c r="AN12" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO12" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP12" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ12" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR12" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="AS11" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT11" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU11" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="AV11" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="AW11" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX11" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY11" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ11" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA11" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB11" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="BC11" s="48" t="s">
+      <c r="AS12" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT12" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU12" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV12" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW12" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX12" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY12" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ12" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA12" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB12" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC12" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="BD12" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="BD11" s="48" t="s">
+      <c r="BE12" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="BE11" s="48" t="s">
+      <c r="BF12" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="BF11" s="48" t="s">
-        <v>229</v>
-      </c>
-      <c r="BG11" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="BH11" s="17" t="s">
+      <c r="BG12" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH12" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:60" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:61" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="52">
+        <f>B11 * 60</f>
+        <v>60</v>
+      </c>
+      <c r="C13" s="52">
+        <f>C11 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="D13" s="52">
+        <f>D11 * 60</f>
+        <v>180</v>
+      </c>
+      <c r="E13" s="52">
+        <f>E11 * 60</f>
+        <v>240</v>
+      </c>
+      <c r="F13" s="52">
+        <f>F11 * 60</f>
+        <v>300</v>
+      </c>
+      <c r="G13" s="53">
+        <f>G11 * 60</f>
+        <v>60</v>
+      </c>
+      <c r="H13" s="53">
+        <f>H11 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="I13" s="53">
+        <f>I11 * 60</f>
+        <v>180</v>
+      </c>
+      <c r="J13" s="53">
+        <f>J11 * 60</f>
+        <v>240</v>
+      </c>
+      <c r="K13" s="53">
+        <f>K11 * 60</f>
+        <v>300</v>
+      </c>
+      <c r="L13" s="54">
+        <f>L11 * 60</f>
+        <v>60</v>
+      </c>
+      <c r="M13" s="54">
+        <f>M11 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="N13" s="54">
+        <f>N11 * 60</f>
+        <v>180</v>
+      </c>
+      <c r="O13" s="54">
+        <f>O11 * 60</f>
+        <v>240</v>
+      </c>
+      <c r="P13" s="54">
+        <f>P11 * 60</f>
+        <v>300</v>
+      </c>
+      <c r="Q13" s="55">
+        <f>Q11 * 60</f>
+        <v>60</v>
+      </c>
+      <c r="R13" s="55">
+        <f>R11 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="S13" s="55">
+        <f>S11 * 60</f>
+        <v>180</v>
+      </c>
+      <c r="T13" s="55">
+        <f>T11 * 60</f>
+        <v>240</v>
+      </c>
+      <c r="U13" s="55">
+        <f>U11 * 60</f>
+        <v>300</v>
+      </c>
+      <c r="V13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="W13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="X13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC13" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD13" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE13" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF13" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG13" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH13" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI13" s="58">
+        <f>AI5 * 60</f>
+        <v>60</v>
+      </c>
+      <c r="AJ13" s="58">
+        <f>AJ5 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="AK13" s="58">
+        <f>AK5 * 60</f>
+        <v>180</v>
+      </c>
+      <c r="AL13" s="58">
+        <f>AL5 * 60</f>
+        <v>240</v>
+      </c>
+      <c r="AM13" s="58">
+        <f>AM5 * 60</f>
+        <v>300</v>
+      </c>
+      <c r="AN13" s="59">
+        <f>AN5 * 60</f>
+        <v>60</v>
+      </c>
+      <c r="AO13" s="59">
+        <f>AO5 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="AP13" s="59">
+        <f>AP5 * 60</f>
+        <v>180</v>
+      </c>
+      <c r="AQ13" s="59">
+        <f>AQ5 * 60</f>
+        <v>240</v>
+      </c>
+      <c r="AR13" s="59">
+        <f>AR5 * 60</f>
+        <v>300</v>
+      </c>
+      <c r="AS13" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT13" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU13" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV13" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW13" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX13" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY13" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ13" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA13" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB13" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC13" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD13" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE13" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF13" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BG13" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH13" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A14" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="52" t="str">
+        <f>B5 * 0.5 * 60 &amp;" IND + " &amp; B5 * 0.5 * 60 &amp; " ISO"</f>
+        <v>30 IND + 30 ISO</v>
+      </c>
+      <c r="C14" s="52" t="str">
+        <f>C5 * 0.5 * 60 &amp;" IND + " &amp; C5 * 0.5 * 60 &amp; " ISO"</f>
+        <v>60 IND + 60 ISO</v>
+      </c>
+      <c r="D14" s="52" t="str">
+        <f>D5 * 0.5 * 60 &amp;" IND + " &amp; D5 * 0.5 * 60 &amp; " ISO"</f>
+        <v>90 IND + 90 ISO</v>
+      </c>
+      <c r="E14" s="52" t="str">
+        <f>E5 * 0.5 * 60 &amp;" IND + " &amp; E5 * 0.5 * 60 &amp; " ISO"</f>
+        <v>120 IND + 120 ISO</v>
+      </c>
+      <c r="F14" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="53" t="str">
+        <f>G5 * 0.75 * 60 &amp;" FOOD"</f>
+        <v>45 FOOD</v>
+      </c>
+      <c r="H14" s="53" t="str">
+        <f>H5 * 0.75 * 60 &amp;" FOOD"</f>
+        <v>90 FOOD</v>
+      </c>
+      <c r="I14" s="53" t="str">
+        <f>I5 * 0.75 * 60 &amp;" FOOD"</f>
+        <v>135 FOOD</v>
+      </c>
+      <c r="J14" s="53" t="str">
+        <f>J5 * 0.75 * 60 &amp;" FOOD"</f>
+        <v>180 FOOD</v>
+      </c>
+      <c r="K14" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="54" t="str">
+        <f>L5* 0.75 * 60&amp;" ISO"</f>
+        <v>45 ISO</v>
+      </c>
+      <c r="M14" s="54" t="str">
+        <f>M5* 0.75 * 60&amp;" ISO"</f>
+        <v>90 ISO</v>
+      </c>
+      <c r="N14" s="54" t="str">
+        <f>N5* 0.75 * 60&amp;" ISO"</f>
+        <v>135 ISO</v>
+      </c>
+      <c r="O14" s="54" t="str">
+        <f>O5* 0.75 * 60&amp;" ISO"</f>
+        <v>180 ISO</v>
+      </c>
+      <c r="P14" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" s="55" t="str">
+        <f>Q5 * 0.5*60 &amp;" FOOD + " &amp;Q5 * 0.75*60 &amp;" IND + "&amp;Q5 * 0.75*60 &amp;" ISO"</f>
+        <v>30 FOOD + 45 IND + 45 ISO</v>
+      </c>
+      <c r="R14" s="55" t="str">
+        <f>R5 * 0.5*60 &amp;" FOOD + " &amp;R5 * 0.75*60 &amp;" IND + "&amp;R5 * 0.75*60 &amp;" ISO"</f>
+        <v>60 FOOD + 90 IND + 90 ISO</v>
+      </c>
+      <c r="S14" s="55" t="str">
+        <f>S5 * 0.5*60 &amp;" FOOD + " &amp;S5 * 0.75*60 &amp;" IND + "&amp;S5 * 0.75*60 &amp;" ISO"</f>
+        <v>90 FOOD + 135 IND + 135 ISO</v>
+      </c>
+      <c r="T14" s="55" t="str">
+        <f>T5 * 0.5*60 &amp;" FOOD + " &amp;T5 * 0.75*60 &amp;" IND + "&amp;T5 * 0.75*60 &amp;" ISO"</f>
+        <v>120 FOOD + 180 IND + 180 ISO</v>
+      </c>
+      <c r="U14" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="V14" s="56" t="s">
+        <v>240</v>
+      </c>
+      <c r="W14" s="56" t="s">
+        <v>241</v>
+      </c>
+      <c r="X14" s="56" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y14" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="Z14" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA14" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB14" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC14" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD14" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE14" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="AF14" s="57" t="s">
+        <v>245</v>
+      </c>
+      <c r="AG14" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="AH14" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI14" s="58" t="str">
+        <f>AI5 *0.5*60&amp;" ISO"</f>
+        <v>30 ISO</v>
+      </c>
+      <c r="AJ14" s="58" t="str">
+        <f>AJ5 *0.5*60&amp;" ISO"</f>
+        <v>60 ISO</v>
+      </c>
+      <c r="AK14" s="58" t="str">
+        <f>AK5 *0.5*60&amp;" ISO"</f>
+        <v>90 ISO</v>
+      </c>
+      <c r="AL14" s="58" t="str">
+        <f>AL5 *0.5*60&amp;" ISO"</f>
+        <v>120 ISO</v>
+      </c>
+      <c r="AM14" s="58" t="str">
+        <f>AM5 *0.5*60&amp;" ISO"</f>
+        <v>150 ISO</v>
+      </c>
+      <c r="AN14" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO14" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP14" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ14" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR14" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX14" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY14" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ14" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA14" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB14" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC14" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="BD14" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="BE14" s="48" t="s">
+        <v>250</v>
+      </c>
+      <c r="BF14" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG14" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH14" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I15" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J15" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L15" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M15" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="N15" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O15" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="P12" s="11" t="s">
+      <c r="P15" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Q12" s="12" t="s">
+      <c r="Q15" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="R12" s="12" t="s">
+      <c r="R15" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="S12" s="12" t="s">
+      <c r="S15" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T12" s="12" t="s">
+      <c r="T15" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="U12" s="12" t="s">
+      <c r="U15" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="V12" s="13" t="s">
+      <c r="V15" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="W12" s="13" t="s">
+      <c r="W15" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X12" s="13" t="s">
+      <c r="X15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="Y12" s="13" t="s">
+      <c r="Y15" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="Z12" s="13" t="s">
+      <c r="Z15" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="AA12" s="13" t="s">
+      <c r="AA15" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="AB12" s="13" t="s">
+      <c r="AB15" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="AC12" s="13" t="s">
+      <c r="AC15" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="14" t="s">
+      <c r="AD15" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="AE12" s="14" t="s">
+      <c r="AE15" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AF12" s="14" t="s">
+      <c r="AF15" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="AG12" s="14" t="s">
+      <c r="AG15" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AH12" s="14" t="s">
+      <c r="AH15" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AI12" s="15" t="s">
+      <c r="AI15" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AJ12" s="15" t="s">
+      <c r="AJ15" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AK12" s="15" t="s">
+      <c r="AK15" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="AL12" s="15" t="s">
+      <c r="AL15" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="AM12" s="15" t="s">
+      <c r="AM15" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="AN12" s="16" t="s">
+      <c r="AN15" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="AO12" s="16" t="s">
+      <c r="AO15" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="AP12" s="16" t="s">
+      <c r="AP15" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="AQ12" s="16" t="s">
+      <c r="AQ15" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="AR12" s="16" t="s">
+      <c r="AR15" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="AS12" s="41" t="s">
+      <c r="AS15" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="AT12" s="41" t="s">
+      <c r="AT15" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="AU12" s="41" t="s">
+      <c r="AU15" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="AV12" s="41" t="s">
+      <c r="AV15" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="AW12" s="41" t="s">
+      <c r="AW15" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="AX12" s="44" t="s">
+      <c r="AX15" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="AY12" s="44" t="s">
+      <c r="AY15" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="AZ12" s="44" t="s">
+      <c r="AZ15" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="BA12" s="44" t="s">
+      <c r="BA15" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="BB12" s="44" t="s">
+      <c r="BB15" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="BC12" s="48" t="s">
+      <c r="BC15" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="BD12" s="48" t="s">
+      <c r="BD15" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="BE12" s="48" t="s">
+      <c r="BE15" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="BF12" s="48" t="s">
+      <c r="BF15" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="BG12" s="48" t="s">
+      <c r="BG15" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="BH12" s="17" t="s">
+      <c r="BH15" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:60" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="16" spans="1:61" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="13" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="W13" s="13" t="s">
+      <c r="W16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="X13" s="13" t="s">
+      <c r="X16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="Y13" s="13" t="s">
+      <c r="Y16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="Z13" s="13" t="s">
+      <c r="Z16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="AA13" s="13" t="s">
+      <c r="AA16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AB13" s="13" t="s">
+      <c r="AB16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AC13" s="13" t="s">
+      <c r="AC16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AD13" s="14" t="s">
+      <c r="AD16" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AE13" s="14" t="s">
+      <c r="AE16" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="AF13" s="14" t="s">
+      <c r="AF16" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="AG13" s="14" t="s">
+      <c r="AG16" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="AH13" s="14" t="s">
+      <c r="AH16" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="15"/>
-      <c r="AK13" s="15"/>
-      <c r="AL13" s="15"/>
-      <c r="AM13" s="15"/>
-      <c r="AN13" s="16"/>
-      <c r="AO13" s="16"/>
-      <c r="AP13" s="16"/>
-      <c r="AQ13" s="16"/>
-      <c r="AR13" s="16"/>
-      <c r="AS13" s="41" t="s">
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="16"/>
+      <c r="AO16" s="16"/>
+      <c r="AP16" s="16"/>
+      <c r="AQ16" s="16"/>
+      <c r="AR16" s="16"/>
+      <c r="AS16" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="AT13" s="41" t="s">
+      <c r="AT16" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="AU13" s="41" t="s">
+      <c r="AU16" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="AV13" s="41" t="s">
+      <c r="AV16" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="AW13" s="41" t="s">
+      <c r="AW16" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="AX13" s="44" t="s">
+      <c r="AX16" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="AY13" s="44" t="s">
+      <c r="AY16" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="AZ13" s="44" t="s">
+      <c r="AZ16" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="BA13" s="44" t="s">
+      <c r="BA16" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="BB13" s="44" t="s">
+      <c r="BB16" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="BC13" s="48" t="s">
+      <c r="BC16" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="BD13" s="48" t="s">
+      <c r="BD16" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="BE13" s="48" t="s">
+      <c r="BE16" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="BF13" s="48" t="s">
+      <c r="BF16" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="BG13" s="48" t="s">
+      <c r="BG16" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="BH13" s="17"/>
+      <c r="BH16" s="17"/>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="F14" s="50" t="s">
+      <c r="F17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="H14" s="50" t="s">
+      <c r="H17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="I14" s="50" t="s">
+      <c r="I17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="J14" s="50" t="s">
+      <c r="J17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="K14" s="50" t="s">
+      <c r="K17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="L14" s="50" t="s">
+      <c r="L17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="M14" s="50" t="s">
+      <c r="M17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="N14" s="50" t="s">
+      <c r="N17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="O14" s="50" t="s">
+      <c r="O17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="P14" s="50" t="s">
+      <c r="P17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="Q14" s="50" t="s">
+      <c r="Q17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="R14" s="50" t="s">
+      <c r="R17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="S14" s="50" t="s">
+      <c r="S17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="T14" s="50" t="s">
+      <c r="T17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="U14" s="50" t="s">
+      <c r="U17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="V14" s="50" t="s">
+      <c r="V17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="W14" s="50" t="s">
+      <c r="W17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="X14" s="50" t="s">
+      <c r="X17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="Y14" s="50" t="s">
+      <c r="Y17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="Z14" s="50" t="s">
+      <c r="Z17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AA14" s="50" t="s">
+      <c r="AA17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AB14" s="50" t="s">
+      <c r="AB17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AC14" s="50" t="s">
+      <c r="AC17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AD14" s="50" t="s">
+      <c r="AD17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AE14" s="50" t="s">
+      <c r="AE17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AF14" s="50" t="s">
+      <c r="AF17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AG14" s="50" t="s">
+      <c r="AG17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AH14" s="50" t="s">
+      <c r="AH17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AI14" s="50" t="s">
+      <c r="AI17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AJ14" s="50" t="s">
+      <c r="AJ17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AK14" s="50" t="s">
+      <c r="AK17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AL14" s="50" t="s">
+      <c r="AL17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AM14" s="50" t="s">
+      <c r="AM17" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AN14" s="50" t="s">
+      <c r="AN17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AO14" s="50" t="s">
+      <c r="AO17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AP14" s="50" t="s">
+      <c r="AP17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AQ14" s="50" t="s">
+      <c r="AQ17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AR14" s="50" t="s">
+      <c r="AR17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AS14" s="50" t="s">
+      <c r="AS17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AT14" s="50" t="s">
+      <c r="AT17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AU14" s="50" t="s">
+      <c r="AU17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AV14" s="50" t="s">
+      <c r="AV17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AW14" s="50" t="s">
+      <c r="AW17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AX14" s="50" t="s">
+      <c r="AX17" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="AY14" s="50" t="s">
+      <c r="AY17" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="AZ14" s="50" t="s">
+      <c r="AZ17" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="BA14" s="50" t="s">
+      <c r="BA17" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="BB14" s="50" t="s">
+      <c r="BB17" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="BC14" s="50" t="s">
+      <c r="BC17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BD14" s="50" t="s">
+      <c r="BD17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BE14" s="50" t="s">
+      <c r="BE17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BF14" s="50" t="s">
+      <c r="BF17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BG14" s="50" t="s">
+      <c r="BG17" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BH14" s="50" t="s">
+      <c r="BH17" s="50" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4122,8 +4856,8 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{6740D5E2-EAC6-40B3-BF7B-A102C82DBF29}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$6,B14)))</xm:f>
-            <xm:f>Tiers!$G$6</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$6,B17)))</xm:f>
+            <xm:f>Tiers!$F$6</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4133,8 +4867,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{73223FEE-7109-41FD-83AD-7C62F00EA6E5}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$5,B14)))</xm:f>
-            <xm:f>Tiers!$G$5</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$5,B17)))</xm:f>
+            <xm:f>Tiers!$F$5</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4144,8 +4878,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{AA3967A1-817B-49EE-83E4-0FA5B7771630}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$4,B14)))</xm:f>
-            <xm:f>Tiers!$G$4</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$4,B17)))</xm:f>
+            <xm:f>Tiers!$F$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4155,8 +4889,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{4F6E6EB3-A34A-46BD-8A7F-3E1A26A40259}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$3,B14)))</xm:f>
-            <xm:f>Tiers!$G$3</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$3,B17)))</xm:f>
+            <xm:f>Tiers!$F$3</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4166,8 +4900,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="5" operator="containsText" id="{98ED36B8-A279-4C77-AB57-9EC7D24FFB6C}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$2,B14)))</xm:f>
-            <xm:f>Tiers!$G$2</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$2,B17)))</xm:f>
+            <xm:f>Tiers!$F$2</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4176,7 +4910,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B14:BH14</xm:sqref>
+          <xm:sqref>B17:BH17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4184,9 +4918,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1EF31FA6-0B72-4669-89A0-DF93CF264664}">
           <x14:formula1>
-            <xm:f>Tiers!$G$2:$G$6</xm:f>
+            <xm:f>Tiers!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B14:BH14</xm:sqref>
+          <xm:sqref>B17:BH17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4905,8 +5639,8 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{ACC789E1-FE5F-4456-A5C8-9F2C1BE04049}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$6,B14)))</xm:f>
-            <xm:f>Tiers!$G$6</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$6,B14)))</xm:f>
+            <xm:f>Tiers!$F$6</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4916,8 +5650,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{25133FF0-E929-4020-8D53-245B6DF69F88}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$5,B14)))</xm:f>
-            <xm:f>Tiers!$G$5</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$5,B14)))</xm:f>
+            <xm:f>Tiers!$F$5</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4927,8 +5661,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{6E0C9BD1-D8C2-4C5D-AFBC-24C38CEED168}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$4,B14)))</xm:f>
-            <xm:f>Tiers!$G$4</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$4,B14)))</xm:f>
+            <xm:f>Tiers!$F$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4938,8 +5672,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{5FEF1AB5-D211-44B9-A883-CD8DC62717E3}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$3,B14)))</xm:f>
-            <xm:f>Tiers!$G$3</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$3,B14)))</xm:f>
+            <xm:f>Tiers!$F$3</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4949,8 +5683,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="5" operator="containsText" id="{10455162-ED76-4B3D-8C86-31C09D66E6EA}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$G$2,B14)))</xm:f>
-            <xm:f>Tiers!$G$2</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$2,B14)))</xm:f>
+            <xm:f>Tiers!$F$2</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4967,7 +5701,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{2DDEC59F-E6EF-4328-B82C-C9A798B9075A}">
           <x14:formula1>
-            <xm:f>Tiers!$G$2:$G$6</xm:f>
+            <xm:f>Tiers!$F$2:$F$6</xm:f>
           </x14:formula1>
           <xm:sqref>B14:O14</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
New assets and testing
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3255F70-1386-4256-90AC-18C1DFDFCE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2919975B-C9C2-442F-A379-4A207FDA508D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="275">
   <si>
     <t>Tier</t>
   </si>
@@ -792,6 +792,75 @@
   </si>
   <si>
     <t>30 FOOD + 120 IND</t>
+  </si>
+  <si>
+    <t>Model Notes</t>
+  </si>
+  <si>
+    <t>A series of small individual garden plots with walkways, lamp posts, and watering/gardening equipment</t>
+  </si>
+  <si>
+    <t>A sizable farm plot with a small shed for tools, a tractor, and a series of farm plants(ie corn, wheat, lettuce)</t>
+  </si>
+  <si>
+    <t>Same as the farm but with fruit trees</t>
+  </si>
+  <si>
+    <t>A large relatively open area with a barn and a couple of farm animals(ie pigs, cows, sheep)</t>
+  </si>
+  <si>
+    <t>A series of hexagonal towers connected by a centeral tower core. Each floor of the hexagonal towers would have plants growing and be semi open air</t>
+  </si>
+  <si>
+    <t>A simple rundown sheet metal shack with a couple of holes, a barely functional door, and a lawn chair out front</t>
+  </si>
+  <si>
+    <t>A simple log cabin with a few potted plants out front and a rocking chair</t>
+  </si>
+  <si>
+    <t>An apartment complex with fire escapes, a simple rooftop access, ac wall units</t>
+  </si>
+  <si>
+    <t>A condo complex with nice glass walls, large balconies and a nice rooftop lounge</t>
+  </si>
+  <si>
+    <t>A very large house with 2-3 floors, a large open area with a pool, a couple of secondary buildings(ie poolhouse, garage, etc) and a privacy wall</t>
+  </si>
+  <si>
+    <t>A simple blacksmith-esque building with various tools and machines scattered around</t>
+  </si>
+  <si>
+    <t>A large, industrial looking machine with metal heating and shaping presses</t>
+  </si>
+  <si>
+    <t>A couple of automation presses with converyor belts and ingedients and products</t>
+  </si>
+  <si>
+    <t>A series of forges connected together with metal ingots scattered about</t>
+  </si>
+  <si>
+    <t>A combination of the previous models connected together to look like a factory</t>
+  </si>
+  <si>
+    <t>A large military style tent with bunkbed racks and foot lockers inside(unnecessary?), work out and military equipment outside</t>
+  </si>
+  <si>
+    <t>A large building with a central open area with work out equipment, a sportsball court, and a military vehicle out front</t>
+  </si>
+  <si>
+    <t>A combination of the previous models and their elements to serve as a more of an organized deployment area</t>
+  </si>
+  <si>
+    <t>A series of small but nice and semi-spartan houses for military officers</t>
+  </si>
+  <si>
+    <t>A large building with various military equipment and satellite dishes scattered about</t>
+  </si>
+  <si>
+    <t>A small building with a couple of gun racks out front with an equal number of alleys and target dummies used for target practice</t>
+  </si>
+  <si>
+    <t>A small building with a training yard that has a number of large tower shields and appropriate training equipment</t>
   </si>
 </sst>
 </file>
@@ -1675,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
-  <dimension ref="A1:BI17"/>
+  <dimension ref="A1:BI18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BI12" sqref="BI12"/>
+    <sheetView tabSelected="1" topLeftCell="R7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -3525,175 +3594,175 @@
         <v>236</v>
       </c>
       <c r="B11" s="31">
-        <f>B5</f>
+        <f t="shared" ref="B11:AR11" si="0">B5</f>
         <v>1</v>
       </c>
       <c r="C11" s="31">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D11" s="31">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E11" s="31">
-        <f>E5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F11" s="31">
-        <f>F5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G11" s="32">
-        <f>G5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H11" s="32">
-        <f>H5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I11" s="32">
-        <f>I5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J11" s="32">
-        <f>J5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K11" s="32">
-        <f>K5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L11" s="33">
-        <f>L5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M11" s="33">
-        <f>M5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N11" s="33">
-        <f>N5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="O11" s="33">
-        <f>O5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P11" s="33">
-        <f>P5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="Q11" s="34">
-        <f>Q5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R11" s="34">
-        <f>R5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="S11" s="34">
-        <f>S5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="T11" s="34">
-        <f>T5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U11" s="34">
-        <f>U5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="V11" s="35" t="str">
-        <f>V5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="W11" s="35" t="str">
-        <f>W5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="X11" s="35" t="str">
-        <f>X5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="Y11" s="35" t="str">
-        <f>Y5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="Z11" s="35" t="str">
-        <f>Z5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AA11" s="35" t="str">
-        <f>AA5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AB11" s="35" t="str">
-        <f>AB5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AC11" s="35" t="str">
-        <f>AC5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AD11" s="30" t="str">
-        <f>AD5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AE11" s="30" t="str">
-        <f>AE5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AF11" s="30" t="str">
-        <f>AF5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AG11" s="30" t="str">
-        <f>AG5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AH11" s="30" t="str">
-        <f>AH5</f>
+        <f t="shared" si="0"/>
         <v>NULL</v>
       </c>
       <c r="AI11" s="36">
-        <f>AI5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AJ11" s="36">
-        <f>AJ5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AK11" s="36">
-        <f>AK5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AL11" s="36">
-        <f>AL5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AM11" s="36">
-        <f>AM5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AN11" s="37">
-        <f>AN5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AO11" s="37">
-        <f>AO5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AP11" s="37">
-        <f>AP5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AQ11" s="37">
-        <f>AQ5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AR11" s="37">
-        <f>AR5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AS11" s="60" t="s">
@@ -3954,83 +4023,83 @@
         <v>237</v>
       </c>
       <c r="B13" s="52">
-        <f>B11 * 60</f>
+        <f t="shared" ref="B13:U13" si="1">B11 * 60</f>
         <v>60</v>
       </c>
       <c r="C13" s="52">
-        <f>C11 * 60</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="D13" s="52">
-        <f>D11 * 60</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="E13" s="52">
-        <f>E11 * 60</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="F13" s="52">
-        <f>F11 * 60</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="G13" s="53">
-        <f>G11 * 60</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H13" s="53">
-        <f>H11 * 60</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="I13" s="53">
-        <f>I11 * 60</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="J13" s="53">
-        <f>J11 * 60</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="K13" s="53">
-        <f>K11 * 60</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="L13" s="54">
-        <f>L11 * 60</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="M13" s="54">
-        <f>M11 * 60</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="N13" s="54">
-        <f>N11 * 60</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="O13" s="54">
-        <f>O11 * 60</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="P13" s="54">
-        <f>P11 * 60</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="Q13" s="55">
-        <f>Q11 * 60</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="R13" s="55">
-        <f>R11 * 60</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="S13" s="55">
-        <f>S11 * 60</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="T13" s="55">
-        <f>T11 * 60</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="U13" s="55">
-        <f>U11 * 60</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="V13" s="56" t="s">
@@ -4073,43 +4142,43 @@
         <v>22</v>
       </c>
       <c r="AI13" s="58">
-        <f>AI5 * 60</f>
+        <f t="shared" ref="AI13:AR13" si="2">AI5 * 60</f>
         <v>60</v>
       </c>
       <c r="AJ13" s="58">
-        <f>AJ5 * 60</f>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="AK13" s="58">
-        <f>AK5 * 60</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AL13" s="58">
-        <f>AL5 * 60</f>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="AM13" s="58">
-        <f>AM5 * 60</f>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="AN13" s="59">
-        <f>AN5 * 60</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="AO13" s="59">
-        <f>AO5 * 60</f>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="AP13" s="59">
-        <f>AP5 * 60</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="AQ13" s="59">
-        <f>AQ5 * 60</f>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="AR13" s="59">
-        <f>AR5 * 60</f>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="AS13" s="60" t="s">
@@ -4666,185 +4735,293 @@
       </c>
       <c r="BH16" s="17"/>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+    <row r="17" spans="1:60" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="U17" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="V17" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="W17" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="14"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
+      <c r="AG17" s="14"/>
+      <c r="AH17" s="14"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="15"/>
+      <c r="AK17" s="15"/>
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="16"/>
+      <c r="AO17" s="16"/>
+      <c r="AP17" s="16"/>
+      <c r="AQ17" s="16"/>
+      <c r="AR17" s="16"/>
+      <c r="AS17" s="41"/>
+      <c r="AT17" s="41"/>
+      <c r="AU17" s="41"/>
+      <c r="AV17" s="41"/>
+      <c r="AW17" s="41"/>
+      <c r="AX17" s="44"/>
+      <c r="AY17" s="44"/>
+      <c r="AZ17" s="44"/>
+      <c r="BA17" s="44"/>
+      <c r="BB17" s="44"/>
+      <c r="BC17" s="48"/>
+      <c r="BD17" s="48"/>
+      <c r="BE17" s="48"/>
+      <c r="BF17" s="48"/>
+      <c r="BG17" s="48"/>
+      <c r="BH17" s="17"/>
+    </row>
+    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="F17" s="50" t="s">
+      <c r="F18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="H17" s="50" t="s">
+      <c r="H18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="I17" s="50" t="s">
+      <c r="I18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="J17" s="50" t="s">
+      <c r="J18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="K17" s="50" t="s">
+      <c r="K18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="L17" s="50" t="s">
+      <c r="L18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="M17" s="50" t="s">
+      <c r="M18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="N17" s="50" t="s">
+      <c r="N18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="O17" s="50" t="s">
+      <c r="O18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="P17" s="50" t="s">
+      <c r="P18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="Q17" s="50" t="s">
+      <c r="Q18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="R17" s="50" t="s">
+      <c r="R18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="S17" s="50" t="s">
+      <c r="S18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="T17" s="50" t="s">
+      <c r="T18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="U17" s="50" t="s">
+      <c r="U18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="V17" s="50" t="s">
+      <c r="V18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="W17" s="50" t="s">
+      <c r="W18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="X17" s="50" t="s">
+      <c r="X18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="Y17" s="50" t="s">
+      <c r="Y18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="Z17" s="50" t="s">
+      <c r="Z18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AA17" s="50" t="s">
+      <c r="AA18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AB17" s="50" t="s">
+      <c r="AB18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AC17" s="50" t="s">
+      <c r="AC18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AD17" s="50" t="s">
+      <c r="AD18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AE17" s="50" t="s">
+      <c r="AE18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AF17" s="50" t="s">
+      <c r="AF18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AG17" s="50" t="s">
+      <c r="AG18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AH17" s="50" t="s">
+      <c r="AH18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AI17" s="50" t="s">
+      <c r="AI18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AJ17" s="50" t="s">
+      <c r="AJ18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AK17" s="50" t="s">
+      <c r="AK18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AL17" s="50" t="s">
+      <c r="AL18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AM17" s="50" t="s">
+      <c r="AM18" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="AN17" s="50" t="s">
+      <c r="AN18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AO17" s="50" t="s">
+      <c r="AO18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AP17" s="50" t="s">
+      <c r="AP18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AQ17" s="50" t="s">
+      <c r="AQ18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AR17" s="50" t="s">
+      <c r="AR18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AS17" s="50" t="s">
+      <c r="AS18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AT17" s="50" t="s">
+      <c r="AT18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AU17" s="50" t="s">
+      <c r="AU18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AV17" s="50" t="s">
+      <c r="AV18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AW17" s="50" t="s">
+      <c r="AW18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AX17" s="50" t="s">
+      <c r="AX18" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="AY17" s="50" t="s">
+      <c r="AY18" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="AZ17" s="50" t="s">
+      <c r="AZ18" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="BA17" s="50" t="s">
+      <c r="BA18" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="BB17" s="50" t="s">
+      <c r="BB18" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="BC17" s="50" t="s">
+      <c r="BC18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BD17" s="50" t="s">
+      <c r="BD18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BE17" s="50" t="s">
+      <c r="BE18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BF17" s="50" t="s">
+      <c r="BF18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BG17" s="50" t="s">
+      <c r="BG18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="BH17" s="50" t="s">
+      <c r="BH18" s="50" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4856,7 +5033,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{6740D5E2-EAC6-40B3-BF7B-A102C82DBF29}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$6,B17)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$6,B18)))</xm:f>
             <xm:f>Tiers!$F$6</xm:f>
             <x14:dxf>
               <fill>
@@ -4867,7 +5044,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{73223FEE-7109-41FD-83AD-7C62F00EA6E5}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$5,B17)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$5,B18)))</xm:f>
             <xm:f>Tiers!$F$5</xm:f>
             <x14:dxf>
               <fill>
@@ -4878,7 +5055,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{AA3967A1-817B-49EE-83E4-0FA5B7771630}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$4,B17)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$4,B18)))</xm:f>
             <xm:f>Tiers!$F$4</xm:f>
             <x14:dxf>
               <fill>
@@ -4889,7 +5066,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{4F6E6EB3-A34A-46BD-8A7F-3E1A26A40259}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$3,B17)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$3,B18)))</xm:f>
             <xm:f>Tiers!$F$3</xm:f>
             <x14:dxf>
               <fill>
@@ -4900,7 +5077,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="5" operator="containsText" id="{98ED36B8-A279-4C77-AB57-9EC7D24FFB6C}">
-            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$2,B17)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Tiers!$F$2,B18)))</xm:f>
             <xm:f>Tiers!$F$2</xm:f>
             <x14:dxf>
               <fill>
@@ -4910,7 +5087,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B17:BH17</xm:sqref>
+          <xm:sqref>B18:BH18</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4920,7 +5097,7 @@
           <x14:formula1>
             <xm:f>Tiers!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B17:BH17</xm:sqref>
+          <xm:sqref>B18:BH18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
still more model work
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC31DFC-433E-4F89-8294-C686C136F84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7276D7-D03D-40EF-A1DA-37658A96F250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" topLeftCell="AE13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK18" sqref="AK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -5120,25 +5120,25 @@
         <v>211</v>
       </c>
       <c r="AD18" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE18" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF18" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="AG18" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH18" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="AE18" s="50" t="s">
+      <c r="AJ18" s="50" t="s">
         <v>211</v>
-      </c>
-      <c r="AF18" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="AG18" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="AH18" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="AI18" s="50" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ18" s="50" t="s">
-        <v>210</v>
       </c>
       <c r="AK18" s="50" t="s">
         <v>210</v>

</xml_diff>

<commit_message>
shader rabbit hole day 2
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE46A767-9F4F-4809-A6AC-EA0070C9EFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7416E779-9464-4ACB-965D-D52E24E44C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR17" sqref="AR17"/>
+    <sheetView tabSelected="1" topLeftCell="AM9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS18" sqref="AS18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -5162,10 +5162,10 @@
         <v>212</v>
       </c>
       <c r="AR18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AS18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AT18" s="50" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
model work is unending
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7416E779-9464-4ACB-965D-D52E24E44C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAFE313-B390-43E1-AC47-28C79310C2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AS18" sqref="AS18"/>
+    <sheetView tabSelected="1" topLeftCell="AW9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BD18" sqref="BD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -5168,16 +5168,16 @@
         <v>212</v>
       </c>
       <c r="AT18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AU18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AV18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AW18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AX18" s="50" t="s">
         <v>212</v>
@@ -5195,7 +5195,7 @@
         <v>212</v>
       </c>
       <c r="BC18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BD18" s="50" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
most model work done
</commit_message>
<xml_diff>
--- a/design docs/Buildings.xlsx
+++ b/design docs/Buildings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hex-trigger\design docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAFE313-B390-43E1-AC47-28C79310C2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0BF399-80F6-48E7-82E5-EA25D3D45A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -1657,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B59688F-6DFE-4C86-8B0D-704C70AF81C9}">
   <dimension ref="A1:BI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BD18" sqref="BD18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BG19" sqref="BG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -5198,19 +5198,19 @@
         <v>212</v>
       </c>
       <c r="BD18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BE18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BF18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BG18" s="50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BH18" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.3">
@@ -5301,7 +5301,7 @@
   <dimension ref="A1:BH14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5936,22 +5936,22 @@
         <v>210</v>
       </c>
       <c r="J14" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K14" s="50" t="s">
         <v>210</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M14" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N14" s="50" t="s">
         <v>210</v>
       </c>
       <c r="O14" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P14" s="50"/>
       <c r="Q14" s="50"/>

</xml_diff>